<commit_message>
Fixed typo in Week 6 Excel example
</commit_message>
<xml_diff>
--- a/Module 2/Week 6 - Diversification and portfolio optimization/Homework 1 example.xlsx
+++ b/Module 2/Week 6 - Diversification and portfolio optimization/Homework 1 example.xlsx
@@ -177,7 +177,7 @@
     <numFmt numFmtId="170" formatCode="0.000000"/>
     <numFmt numFmtId="171" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -207,19 +207,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="13"/>
@@ -295,7 +282,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -328,15 +315,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -352,10 +335,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -368,15 +347,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -456,7 +435,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -485,8 +464,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.313854527461653"/>
-          <c:y val="0.0351864883884588"/>
+          <c:x val="0.313818487228892"/>
+          <c:y val="0.0352775578428785"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -545,6 +524,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -890,11 +870,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="15159247"/>
-        <c:axId val="73528769"/>
+        <c:axId val="71963995"/>
+        <c:axId val="7238758"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="15159247"/>
+        <c:axId val="71963995"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -928,7 +908,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -950,12 +930,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73528769"/>
+        <c:crossAx val="7238758"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73528769"/>
+        <c:axId val="7238758"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.006"/>
@@ -999,7 +979,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1021,9 +1001,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15159247"/>
+        <c:crossAx val="71963995"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1048,7 +1028,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1077,8 +1057,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.313877307921382"/>
-          <c:y val="0.0353833936292244"/>
+          <c:x val="0.313890678428069"/>
+          <c:y val="0.0354747617366749"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1137,6 +1117,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1514,6 +1495,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1551,154 +1533,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000710296041441044</c:v>
+                  <c:v>0.0007115265690196</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00142059208288209</c:v>
+                  <c:v>0.0014230531380392</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.00213088812432313</c:v>
+                  <c:v>0.0021345797070588</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00284118416576417</c:v>
+                  <c:v>0.0028461062760784</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.00355148020720522</c:v>
+                  <c:v>0.003557632845098</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00426177624864626</c:v>
+                  <c:v>0.0042691594141176</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.00497207229008731</c:v>
+                  <c:v>0.0049806859831372</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.00568236833152835</c:v>
+                  <c:v>0.0056922125521568</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.00639266437296939</c:v>
+                  <c:v>0.0064037391211764</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.00710296041441044</c:v>
+                  <c:v>0.007115265690196</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.00781325645585148</c:v>
+                  <c:v>0.0078267922592156</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.00852355249729252</c:v>
+                  <c:v>0.0085383188282352</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.00923384853873357</c:v>
+                  <c:v>0.0092498453972548</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.00994414458017461</c:v>
+                  <c:v>0.0099613719662744</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0106544406216157</c:v>
+                  <c:v>0.010672898535294</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.0113647366630567</c:v>
+                  <c:v>0.0113844251043136</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.0120750327044977</c:v>
+                  <c:v>0.0120959516733332</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.0127853287459388</c:v>
+                  <c:v>0.0128074782423528</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.0134956247873798</c:v>
+                  <c:v>0.0135190048113724</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.0142059208288209</c:v>
+                  <c:v>0.014230531380392</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.0149162168702619</c:v>
+                  <c:v>0.0149420579494116</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.015626512911703</c:v>
+                  <c:v>0.0156535845184312</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.016336808953144</c:v>
+                  <c:v>0.0163651110874508</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.0170471049945851</c:v>
+                  <c:v>0.0170766376564704</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0177574010360261</c:v>
+                  <c:v>0.01778816422549</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0184676970774671</c:v>
+                  <c:v>0.0184996907945096</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.0191779931189082</c:v>
+                  <c:v>0.0192112173635292</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.0198882891603492</c:v>
+                  <c:v>0.0199227439325488</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.0205985852017903</c:v>
+                  <c:v>0.0206342705015684</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.0213088812432313</c:v>
+                  <c:v>0.021345797070588</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0220191772846724</c:v>
+                  <c:v>0.0220573236396076</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.0227294733261134</c:v>
+                  <c:v>0.0227688502086272</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.0234397693675545</c:v>
+                  <c:v>0.0234803767776468</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.0241500654089955</c:v>
+                  <c:v>0.0241919033466664</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.0248603614504365</c:v>
+                  <c:v>0.024903429915686</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.0255706574918776</c:v>
+                  <c:v>0.0256149564847056</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.0262809535333186</c:v>
+                  <c:v>0.0263264830537252</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.0269912495747597</c:v>
+                  <c:v>0.0270380096227448</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.0277015456162007</c:v>
+                  <c:v>0.0277495361917644</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.0284118416576418</c:v>
+                  <c:v>0.028461062760784</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.0291221376990828</c:v>
+                  <c:v>0.0291725893298036</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.0298324337405239</c:v>
+                  <c:v>0.0298841158988232</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.0305427297819649</c:v>
+                  <c:v>0.0305956424678428</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.0312530258234059</c:v>
+                  <c:v>0.0313071690368624</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.031963321864847</c:v>
+                  <c:v>0.032018695605882</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.032673617906288</c:v>
+                  <c:v>0.0327302221749016</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.0333839139477291</c:v>
+                  <c:v>0.0334417487439212</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.0340942099891701</c:v>
+                  <c:v>0.0341532753129408</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.0348045060306112</c:v>
+                  <c:v>0.0348648018819604</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.0355148020720522</c:v>
+                  <c:v>0.03557632845098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1713,165 +1695,165 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000141009684317938</c:v>
+                  <c:v>0.000141300103443267</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000282019368635876</c:v>
+                  <c:v>0.000282600206886534</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.000423029052953815</c:v>
+                  <c:v>0.000423900310329802</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.000564038737271753</c:v>
+                  <c:v>0.000565200413773069</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.000705048421589691</c:v>
+                  <c:v>0.000706500517216336</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00084605810590763</c:v>
+                  <c:v>0.000847800620659603</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.000987067790225568</c:v>
+                  <c:v>0.00098910072410287</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.00112807747454351</c:v>
+                  <c:v>0.00113040082754614</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.00126908715886144</c:v>
+                  <c:v>0.0012717009309894</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.00141009684317938</c:v>
+                  <c:v>0.00141300103443267</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.00155110652749732</c:v>
+                  <c:v>0.00155430113787594</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.00169211621181526</c:v>
+                  <c:v>0.00169560124131921</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0018331258961332</c:v>
+                  <c:v>0.00183690134476247</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.00197413558045114</c:v>
+                  <c:v>0.00197820144820574</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.00211514526476907</c:v>
+                  <c:v>0.00211950155164901</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.00225615494908701</c:v>
+                  <c:v>0.00226080165509228</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.00239716463340495</c:v>
+                  <c:v>0.00240210175853554</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.00253817431772289</c:v>
+                  <c:v>0.00254340186197881</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.00267918400204083</c:v>
+                  <c:v>0.00268470196542208</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.00282019368635877</c:v>
+                  <c:v>0.00282600206886534</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.0029612033706767</c:v>
+                  <c:v>0.00296730217230861</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.00310221305499464</c:v>
+                  <c:v>0.00310860227575188</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.00324322273931258</c:v>
+                  <c:v>0.00324990237919515</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.00338423242363052</c:v>
+                  <c:v>0.00339120248263841</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.00352524210794846</c:v>
+                  <c:v>0.00353250258608168</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0036662517922664</c:v>
+                  <c:v>0.00367380268952495</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.00380726147658433</c:v>
+                  <c:v>0.00381510279296821</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.00394827116090227</c:v>
+                  <c:v>0.00395640289641148</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.00408928084522021</c:v>
+                  <c:v>0.00409770299985475</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.00423029052953815</c:v>
+                  <c:v>0.00423900310329802</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.00437130021385609</c:v>
+                  <c:v>0.00438030320674128</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.00451230989817403</c:v>
+                  <c:v>0.00452160331018455</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.00465331958249196</c:v>
+                  <c:v>0.00466290341362782</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.0047943292668099</c:v>
+                  <c:v>0.00480420351707109</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.00493533895112784</c:v>
+                  <c:v>0.00494550362051435</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.00507634863544578</c:v>
+                  <c:v>0.00508680372395762</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.00521735831976372</c:v>
+                  <c:v>0.00522810382740089</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.00535836800408166</c:v>
+                  <c:v>0.00536940393084415</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.00549937768839959</c:v>
+                  <c:v>0.00551070403428742</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.00564038737271753</c:v>
+                  <c:v>0.00565200413773069</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.00578139705703547</c:v>
+                  <c:v>0.00579330424117395</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.00592240674135341</c:v>
+                  <c:v>0.00593460434461722</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.00606341642567135</c:v>
+                  <c:v>0.00607590444806049</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.00620442610998929</c:v>
+                  <c:v>0.00621720455150376</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.00634543579430722</c:v>
+                  <c:v>0.00635850465494702</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.00648644547862516</c:v>
+                  <c:v>0.00649980475839029</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.0066274551629431</c:v>
+                  <c:v>0.00664110486183356</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.00676846484726104</c:v>
+                  <c:v>0.00678240496527683</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.00690947453157898</c:v>
+                  <c:v>0.00692370506872009</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.00705048421589692</c:v>
+                  <c:v>0.00706500517216336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="92759522"/>
-        <c:axId val="6246711"/>
+        <c:axId val="71971695"/>
+        <c:axId val="13234067"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92759522"/>
+        <c:axId val="71971695"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1905,7 +1887,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1927,12 +1909,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6246711"/>
+        <c:crossAx val="13234067"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="6246711"/>
+        <c:axId val="13234067"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1976,7 +1958,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1998,9 +1980,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92759522"/>
+        <c:crossAx val="71971695"/>
         <c:crossesAt val="0"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2036,9 +2018,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
+      <xdr:colOff>380520</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:rowOff>48600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2047,7 +2029,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6747840" y="163080"/>
-        <a:ext cx="7275240" cy="4092120"/>
+        <a:ext cx="7286400" cy="4091760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2066,9 +2048,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>352080</xdr:colOff>
+      <xdr:colOff>351720</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>9720</xdr:rowOff>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2077,7 +2059,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6741360" y="4342680"/>
-        <a:ext cx="7252920" cy="4079520"/>
+        <a:ext cx="7264080" cy="4079160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2098,12 +2080,12 @@
   <dimension ref="A1:B242"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O8" activeCellId="0" sqref="O8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4060,7 +4042,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
   </cols>
@@ -4069,13 +4051,13 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -8186,10 +8168,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="19.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="24.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10876,10 +10858,10 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="19.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="24.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13566,10 +13548,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16256,7 +16238,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="11.52"/>
@@ -20383,7 +20365,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
   </cols>
@@ -24506,10 +24488,10 @@
   <dimension ref="A1:G118"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.24"/>
@@ -24591,21 +24573,21 @@
       <c r="C10" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="10" t="n">
+      <c r="B11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8" t="n">
         <f aca="false">1-B11</f>
         <v>1</v>
       </c>
@@ -24617,17 +24599,17 @@
         <f aca="false">B11*B$3 + C11*C$3</f>
         <v>0.0081105140233472</v>
       </c>
-      <c r="F11" s="12" t="n">
+      <c r="F11" s="11" t="n">
         <f aca="false">E11/D11</f>
         <v>0.133586241031701</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="10" t="n">
+      <c r="B12" s="8" t="n">
         <f aca="false">B11+0.02</f>
         <v>0.02</v>
       </c>
-      <c r="C12" s="10" t="n">
+      <c r="C12" s="8" t="n">
         <f aca="false">1-B12</f>
         <v>0.98</v>
       </c>
@@ -24639,17 +24621,17 @@
         <f aca="false">B12*B$3 + C12*C$3</f>
         <v>0.00808147211081432</v>
       </c>
-      <c r="F12" s="12" t="n">
+      <c r="F12" s="11" t="n">
         <f aca="false">E12/D12</f>
         <v>0.13539191747862</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10" t="n">
+      <c r="B13" s="8" t="n">
         <f aca="false">B12+0.02</f>
         <v>0.04</v>
       </c>
-      <c r="C13" s="10" t="n">
+      <c r="C13" s="8" t="n">
         <f aca="false">1-B13</f>
         <v>0.96</v>
       </c>
@@ -24661,17 +24643,17 @@
         <f aca="false">B13*B$3 + C13*C$3</f>
         <v>0.00805243019828143</v>
       </c>
-      <c r="F13" s="12" t="n">
+      <c r="F13" s="11" t="n">
         <f aca="false">E13/D13</f>
         <v>0.137238579006424</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10" t="n">
+      <c r="B14" s="8" t="n">
         <f aca="false">B13+0.02</f>
         <v>0.06</v>
       </c>
-      <c r="C14" s="10" t="n">
+      <c r="C14" s="8" t="n">
         <f aca="false">1-B14</f>
         <v>0.94</v>
       </c>
@@ -24683,17 +24665,17 @@
         <f aca="false">B14*B$3 + C14*C$3</f>
         <v>0.00802338828574855</v>
       </c>
-      <c r="F14" s="12" t="n">
+      <c r="F14" s="11" t="n">
         <f aca="false">E14/D14</f>
         <v>0.139126281949099</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10" t="n">
+      <c r="B15" s="8" t="n">
         <f aca="false">B14+0.02</f>
         <v>0.08</v>
       </c>
-      <c r="C15" s="10" t="n">
+      <c r="C15" s="8" t="n">
         <f aca="false">1-B15</f>
         <v>0.92</v>
       </c>
@@ -24705,17 +24687,17 @@
         <f aca="false">B15*B$3 + C15*C$3</f>
         <v>0.00799434637321566</v>
       </c>
-      <c r="F15" s="12" t="n">
+      <c r="F15" s="11" t="n">
         <f aca="false">E15/D15</f>
         <v>0.141054902577417</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="10" t="n">
+      <c r="B16" s="8" t="n">
         <f aca="false">B15+0.02</f>
         <v>0.1</v>
       </c>
-      <c r="C16" s="10" t="n">
+      <c r="C16" s="8" t="n">
         <f aca="false">1-B16</f>
         <v>0.9</v>
       </c>
@@ -24727,17 +24709,17 @@
         <f aca="false">B16*B$3 + C16*C$3</f>
         <v>0.00796530446068278</v>
       </c>
-      <c r="F16" s="12" t="n">
+      <c r="F16" s="11" t="n">
         <f aca="false">E16/D16</f>
         <v>0.143024107549581</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="10" t="n">
+      <c r="B17" s="8" t="n">
         <f aca="false">B16+0.02</f>
         <v>0.12</v>
       </c>
-      <c r="C17" s="10" t="n">
+      <c r="C17" s="8" t="n">
         <f aca="false">1-B17</f>
         <v>0.88</v>
       </c>
@@ -24749,17 +24731,17 @@
         <f aca="false">B17*B$3 + C17*C$3</f>
         <v>0.00793626254814989</v>
       </c>
-      <c r="F17" s="12" t="n">
+      <c r="F17" s="11" t="n">
         <f aca="false">E17/D17</f>
         <v>0.14503332092143</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="10" t="n">
+      <c r="B18" s="8" t="n">
         <f aca="false">B17+0.02</f>
         <v>0.14</v>
       </c>
-      <c r="C18" s="10" t="n">
+      <c r="C18" s="8" t="n">
         <f aca="false">1-B18</f>
         <v>0.86</v>
       </c>
@@ -24771,17 +24753,17 @@
         <f aca="false">B18*B$3 + C18*C$3</f>
         <v>0.00790722063561701</v>
       </c>
-      <c r="F18" s="12" t="n">
+      <c r="F18" s="11" t="n">
         <f aca="false">E18/D18</f>
         <v>0.147081687496546</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="10" t="n">
+      <c r="B19" s="8" t="n">
         <f aca="false">B18+0.02</f>
         <v>0.16</v>
       </c>
-      <c r="C19" s="10" t="n">
+      <c r="C19" s="8" t="n">
         <f aca="false">1-B19</f>
         <v>0.84</v>
       </c>
@@ -24793,17 +24775,17 @@
         <f aca="false">B19*B$3 + C19*C$3</f>
         <v>0.00787817872308412</v>
       </c>
-      <c r="F19" s="12" t="n">
+      <c r="F19" s="11" t="n">
         <f aca="false">E19/D19</f>
         <v>0.149168032333235</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="10" t="n">
+      <c r="B20" s="8" t="n">
         <f aca="false">B19+0.02</f>
         <v>0.18</v>
       </c>
-      <c r="C20" s="10" t="n">
+      <c r="C20" s="8" t="n">
         <f aca="false">1-B20</f>
         <v>0.82</v>
       </c>
@@ -24815,17 +24797,17 @@
         <f aca="false">B20*B$3 + C20*C$3</f>
         <v>0.00784913681055124</v>
       </c>
-      <c r="F20" s="12" t="n">
+      <c r="F20" s="11" t="n">
         <f aca="false">E20/D20</f>
         <v>0.151290816281715</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="10" t="n">
+      <c r="B21" s="8" t="n">
         <f aca="false">B20+0.02</f>
         <v>0.2</v>
       </c>
-      <c r="C21" s="10" t="n">
+      <c r="C21" s="8" t="n">
         <f aca="false">1-B21</f>
         <v>0.8</v>
       </c>
@@ -24837,17 +24819,17 @@
         <f aca="false">B21*B$3 + C21*C$3</f>
         <v>0.00782009489801835</v>
       </c>
-      <c r="F21" s="12" t="n">
+      <c r="F21" s="11" t="n">
         <f aca="false">E21/D21</f>
         <v>0.153448087505689</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="10" t="n">
+      <c r="B22" s="8" t="n">
         <f aca="false">B21+0.02</f>
         <v>0.22</v>
       </c>
-      <c r="C22" s="10" t="n">
+      <c r="C22" s="8" t="n">
         <f aca="false">1-B22</f>
         <v>0.78</v>
       </c>
@@ -24859,17 +24841,17 @@
         <f aca="false">B22*B$3 + C22*C$3</f>
         <v>0.00779105298548547</v>
       </c>
-      <c r="F22" s="12" t="n">
+      <c r="F22" s="11" t="n">
         <f aca="false">E22/D22</f>
         <v>0.155637429053688</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="10" t="n">
+      <c r="B23" s="8" t="n">
         <f aca="false">B22+0.02</f>
         <v>0.24</v>
       </c>
-      <c r="C23" s="10" t="n">
+      <c r="C23" s="8" t="n">
         <f aca="false">1-B23</f>
         <v>0.76</v>
       </c>
@@ -24881,17 +24863,17 @@
         <f aca="false">B23*B$3 + C23*C$3</f>
         <v>0.00776201107295258</v>
       </c>
-      <c r="F23" s="12" t="n">
+      <c r="F23" s="11" t="n">
         <f aca="false">E23/D23</f>
         <v>0.157855902693077</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="10" t="n">
+      <c r="B24" s="8" t="n">
         <f aca="false">B23+0.02</f>
         <v>0.26</v>
       </c>
-      <c r="C24" s="10" t="n">
+      <c r="C24" s="8" t="n">
         <f aca="false">1-B24</f>
         <v>0.74</v>
       </c>
@@ -24903,17 +24885,17 @@
         <f aca="false">B24*B$3 + C24*C$3</f>
         <v>0.0077329691604197</v>
       </c>
-      <c r="F24" s="12" t="n">
+      <c r="F24" s="11" t="n">
         <f aca="false">E24/D24</f>
         <v>0.160099989410032</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="10" t="n">
+      <c r="B25" s="8" t="n">
         <f aca="false">B24+0.02</f>
         <v>0.28</v>
       </c>
-      <c r="C25" s="10" t="n">
+      <c r="C25" s="8" t="n">
         <f aca="false">1-B25</f>
         <v>0.72</v>
       </c>
@@ -24925,17 +24907,17 @@
         <f aca="false">B25*B$3 + C25*C$3</f>
         <v>0.00770392724788682</v>
       </c>
-      <c r="F25" s="12" t="n">
+      <c r="F25" s="11" t="n">
         <f aca="false">E25/D25</f>
         <v>0.162365527218389</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="10" t="n">
+      <c r="B26" s="8" t="n">
         <f aca="false">B25+0.02</f>
         <v>0.3</v>
       </c>
-      <c r="C26" s="10" t="n">
+      <c r="C26" s="8" t="n">
         <f aca="false">1-B26</f>
         <v>0.7</v>
       </c>
@@ -24947,17 +24929,17 @@
         <f aca="false">B26*B$3 + C26*C$3</f>
         <v>0.00767488533535393</v>
       </c>
-      <c r="F26" s="12" t="n">
+      <c r="F26" s="11" t="n">
         <f aca="false">E26/D26</f>
         <v>0.164647647214705</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="10" t="n">
+      <c r="B27" s="8" t="n">
         <f aca="false">B26+0.02</f>
         <v>0.32</v>
       </c>
-      <c r="C27" s="10" t="n">
+      <c r="C27" s="8" t="n">
         <f aca="false">1-B27</f>
         <v>0.68</v>
       </c>
@@ -24969,17 +24951,17 @@
         <f aca="false">B27*B$3 + C27*C$3</f>
         <v>0.00764584342282105</v>
       </c>
-      <c r="F27" s="12" t="n">
+      <c r="F27" s="11" t="n">
         <f aca="false">E27/D27</f>
         <v>0.166940709170115</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="10" t="n">
+      <c r="B28" s="8" t="n">
         <f aca="false">B27+0.02</f>
         <v>0.34</v>
       </c>
-      <c r="C28" s="10" t="n">
+      <c r="C28" s="8" t="n">
         <f aca="false">1-B28</f>
         <v>0.66</v>
       </c>
@@ -24991,17 +24973,17 @@
         <f aca="false">B28*B$3 + C28*C$3</f>
         <v>0.00761680151028816</v>
       </c>
-      <c r="F28" s="12" t="n">
+      <c r="F28" s="11" t="n">
         <f aca="false">E28/D28</f>
         <v>0.169238238362901</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="10" t="n">
+      <c r="B29" s="8" t="n">
         <f aca="false">B28+0.02</f>
         <v>0.36</v>
       </c>
-      <c r="C29" s="10" t="n">
+      <c r="C29" s="8" t="n">
         <f aca="false">1-B29</f>
         <v>0.64</v>
       </c>
@@ -25013,17 +24995,17 @@
         <f aca="false">B29*B$3 + C29*C$3</f>
         <v>0.00758775959775528</v>
       </c>
-      <c r="F29" s="12" t="n">
+      <c r="F29" s="11" t="n">
         <f aca="false">E29/D29</f>
         <v>0.171532865825914</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="10" t="n">
+      <c r="B30" s="8" t="n">
         <f aca="false">B29+0.02</f>
         <v>0.38</v>
       </c>
-      <c r="C30" s="10" t="n">
+      <c r="C30" s="8" t="n">
         <f aca="false">1-B30</f>
         <v>0.62</v>
       </c>
@@ -25035,17 +25017,17 @@
         <f aca="false">B30*B$3 + C30*C$3</f>
         <v>0.00755871768522239</v>
       </c>
-      <c r="F30" s="12" t="n">
+      <c r="F30" s="11" t="n">
         <f aca="false">E30/D30</f>
         <v>0.173816274700855</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="10" t="n">
+      <c r="B31" s="8" t="n">
         <f aca="false">B30+0.02</f>
         <v>0.4</v>
       </c>
-      <c r="C31" s="10" t="n">
+      <c r="C31" s="8" t="n">
         <f aca="false">1-B31</f>
         <v>0.6</v>
       </c>
@@ -25057,17 +25039,17 @@
         <f aca="false">B31*B$3 + C31*C$3</f>
         <v>0.00752967577268951</v>
       </c>
-      <c r="F31" s="12" t="n">
+      <c r="F31" s="11" t="n">
         <f aca="false">E31/D31</f>
         <v>0.176079155939262</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="10" t="n">
+      <c r="B32" s="8" t="n">
         <f aca="false">B31+0.02</f>
         <v>0.42</v>
       </c>
-      <c r="C32" s="10" t="n">
+      <c r="C32" s="8" t="n">
         <f aca="false">1-B32</f>
         <v>0.58</v>
       </c>
@@ -25079,17 +25061,17 @@
         <f aca="false">B32*B$3 + C32*C$3</f>
         <v>0.00750063386015662</v>
       </c>
-      <c r="F32" s="12" t="n">
+      <c r="F32" s="11" t="n">
         <f aca="false">E32/D32</f>
         <v>0.178311177139779</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="10" t="n">
+      <c r="B33" s="8" t="n">
         <f aca="false">B32+0.02</f>
         <v>0.44</v>
       </c>
-      <c r="C33" s="10" t="n">
+      <c r="C33" s="8" t="n">
         <f aca="false">1-B33</f>
         <v>0.56</v>
       </c>
@@ -25101,17 +25083,17 @@
         <f aca="false">B33*B$3 + C33*C$3</f>
         <v>0.00747159194762374</v>
       </c>
-      <c r="F33" s="12" t="n">
+      <c r="F33" s="11" t="n">
         <f aca="false">E33/D33</f>
         <v>0.180500968822188</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="10" t="n">
+      <c r="B34" s="8" t="n">
         <f aca="false">B33+0.02</f>
         <v>0.46</v>
       </c>
-      <c r="C34" s="10" t="n">
+      <c r="C34" s="8" t="n">
         <f aca="false">1-B34</f>
         <v>0.54</v>
       </c>
@@ -25123,17 +25105,17 @@
         <f aca="false">B34*B$3 + C34*C$3</f>
         <v>0.00744255003509085</v>
       </c>
-      <c r="F34" s="12" t="n">
+      <c r="F34" s="11" t="n">
         <f aca="false">E34/D34</f>
         <v>0.18263613285642</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="10" t="n">
+      <c r="B35" s="8" t="n">
         <f aca="false">B34+0.02</f>
         <v>0.48</v>
       </c>
-      <c r="C35" s="10" t="n">
+      <c r="C35" s="8" t="n">
         <f aca="false">1-B35</f>
         <v>0.52</v>
       </c>
@@ -25145,17 +25127,17 @@
         <f aca="false">B35*B$3 + C35*C$3</f>
         <v>0.00741350812255797</v>
       </c>
-      <c r="F35" s="12" t="n">
+      <c r="F35" s="11" t="n">
         <f aca="false">E35/D35</f>
         <v>0.184703278020741</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="10" t="n">
+      <c r="B36" s="8" t="n">
         <f aca="false">B35+0.02</f>
         <v>0.5</v>
       </c>
-      <c r="C36" s="10" t="n">
+      <c r="C36" s="8" t="n">
         <f aca="false">1-B36</f>
         <v>0.5</v>
       </c>
@@ -25167,17 +25149,17 @@
         <f aca="false">B36*B$3 + C36*C$3</f>
         <v>0.00738446621002509</v>
       </c>
-      <c r="F36" s="12" t="n">
+      <c r="F36" s="11" t="n">
         <f aca="false">E36/D36</f>
         <v>0.18668808767722</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="10" t="n">
+      <c r="B37" s="8" t="n">
         <f aca="false">B36+0.02</f>
         <v>0.52</v>
       </c>
-      <c r="C37" s="10" t="n">
+      <c r="C37" s="8" t="n">
         <f aca="false">1-B37</f>
         <v>0.48</v>
       </c>
@@ -25189,17 +25171,17 @@
         <f aca="false">B37*B$3 + C37*C$3</f>
         <v>0.0073554242974922</v>
       </c>
-      <c r="F37" s="12" t="n">
+      <c r="F37" s="11" t="n">
         <f aca="false">E37/D37</f>
         <v>0.188575424236538</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="10" t="n">
+      <c r="B38" s="8" t="n">
         <f aca="false">B37+0.02</f>
         <v>0.54</v>
       </c>
-      <c r="C38" s="10" t="n">
+      <c r="C38" s="8" t="n">
         <f aca="false">1-B38</f>
         <v>0.46</v>
       </c>
@@ -25211,17 +25193,17 @@
         <f aca="false">B38*B$3 + C38*C$3</f>
         <v>0.00732638238495932</v>
       </c>
-      <c r="F38" s="12" t="n">
+      <c r="F38" s="11" t="n">
         <f aca="false">E38/D38</f>
         <v>0.190349474351269</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="10" t="n">
+      <c r="B39" s="8" t="n">
         <f aca="false">B38+0.02</f>
         <v>0.56</v>
       </c>
-      <c r="C39" s="10" t="n">
+      <c r="C39" s="8" t="n">
         <f aca="false">1-B39</f>
         <v>0.44</v>
       </c>
@@ -25233,17 +25215,17 @@
         <f aca="false">B39*B$3 + C39*C$3</f>
         <v>0.00729734047242643</v>
       </c>
-      <c r="F39" s="12" t="n">
+      <c r="F39" s="11" t="n">
         <f aca="false">E39/D39</f>
         <v>0.191993937552701</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="10" t="n">
+      <c r="B40" s="8" t="n">
         <f aca="false">B39+0.02</f>
         <v>0.58</v>
       </c>
-      <c r="C40" s="10" t="n">
+      <c r="C40" s="8" t="n">
         <f aca="false">1-B40</f>
         <v>0.42</v>
       </c>
@@ -25255,17 +25237,17 @@
         <f aca="false">B40*B$3 + C40*C$3</f>
         <v>0.00726829855989355</v>
       </c>
-      <c r="F40" s="12" t="n">
+      <c r="F40" s="11" t="n">
         <f aca="false">E40/D40</f>
         <v>0.193492259285057</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="10" t="n">
+      <c r="B41" s="8" t="n">
         <f aca="false">B40+0.02</f>
         <v>0.6</v>
       </c>
-      <c r="C41" s="10" t="n">
+      <c r="C41" s="8" t="n">
         <f aca="false">1-B41</f>
         <v>0.4</v>
       </c>
@@ -25277,17 +25259,17 @@
         <f aca="false">B41*B$3 + C41*C$3</f>
         <v>0.00723925664736066</v>
       </c>
-      <c r="F41" s="12" t="n">
+      <c r="F41" s="11" t="n">
         <f aca="false">E41/D41</f>
         <v>0.194827906992498</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="10" t="n">
+      <c r="B42" s="8" t="n">
         <f aca="false">B41+0.02</f>
         <v>0.62</v>
       </c>
-      <c r="C42" s="10" t="n">
+      <c r="C42" s="8" t="n">
         <f aca="false">1-B42</f>
         <v>0.38</v>
       </c>
@@ -25299,17 +25281,17 @@
         <f aca="false">B42*B$3 + C42*C$3</f>
         <v>0.00721021473482778</v>
       </c>
-      <c r="F42" s="12" t="n">
+      <c r="F42" s="11" t="n">
         <f aca="false">E42/D42</f>
         <v>0.195984685141562</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="10" t="n">
+      <c r="B43" s="8" t="n">
         <f aca="false">B42+0.02</f>
         <v>0.64</v>
       </c>
-      <c r="C43" s="10" t="n">
+      <c r="C43" s="8" t="n">
         <f aca="false">1-B43</f>
         <v>0.36</v>
       </c>
@@ -25321,17 +25303,17 @@
         <f aca="false">B43*B$3 + C43*C$3</f>
         <v>0.00718117282229489</v>
       </c>
-      <c r="F43" s="12" t="n">
+      <c r="F43" s="11" t="n">
         <f aca="false">E43/D43</f>
         <v>0.196947081954681</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="10" t="n">
+      <c r="B44" s="8" t="n">
         <f aca="false">B43+0.02</f>
         <v>0.66</v>
       </c>
-      <c r="C44" s="10" t="n">
+      <c r="C44" s="8" t="n">
         <f aca="false">1-B44</f>
         <v>0.34</v>
       </c>
@@ -25343,17 +25325,17 @@
         <f aca="false">B44*B$3 + C44*C$3</f>
         <v>0.00715213090976201</v>
       </c>
-      <c r="F44" s="12" t="n">
+      <c r="F44" s="11" t="n">
         <f aca="false">E44/D44</f>
         <v>0.197700637410726</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="10" t="n">
+      <c r="B45" s="8" t="n">
         <f aca="false">B44+0.02</f>
         <v>0.68</v>
       </c>
-      <c r="C45" s="10" t="n">
+      <c r="C45" s="8" t="n">
         <f aca="false">1-B45</f>
         <v>0.32</v>
       </c>
@@ -25365,17 +25347,17 @@
         <f aca="false">B45*B$3 + C45*C$3</f>
         <v>0.00712308899722912</v>
       </c>
-      <c r="F45" s="12" t="n">
+      <c r="F45" s="11" t="n">
         <f aca="false">E45/D45</f>
         <v>0.198232319032442</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="10" t="n">
+      <c r="B46" s="8" t="n">
         <f aca="false">B45+0.02</f>
         <v>0.7</v>
       </c>
-      <c r="C46" s="10" t="n">
+      <c r="C46" s="8" t="n">
         <f aca="false">1-B46</f>
         <v>0.3</v>
       </c>
@@ -25387,38 +25369,38 @@
         <f aca="false">B46*B$3 + C46*C$3</f>
         <v>0.00709404708469624</v>
       </c>
-      <c r="F46" s="12" t="n">
+      <c r="F46" s="11" t="n">
         <f aca="false">E46/D46</f>
         <v>0.19853088947502</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="13" t="n">
+      <c r="B47" s="12" t="n">
         <f aca="false">B46+0.02</f>
         <v>0.72</v>
       </c>
-      <c r="C47" s="13" t="n">
+      <c r="C47" s="12" t="n">
         <f aca="false">1-B47</f>
         <v>0.28</v>
       </c>
-      <c r="D47" s="14" t="n">
+      <c r="D47" s="12" t="n">
         <f aca="false">SQRT( B47^2*B$4^2 + C47^2*C$4^2 + 2*B47*C47*B$6)</f>
         <v>0.03557632845098</v>
       </c>
-      <c r="E47" s="14" t="n">
+      <c r="E47" s="12" t="n">
         <f aca="false">B47*B$3 + C47*C$3</f>
         <v>0.00706500517216336</v>
       </c>
-      <c r="F47" s="15" t="n">
+      <c r="F47" s="13" t="n">
         <f aca="false">E47/D47</f>
         <v>0.198587248313105</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="10" t="n">
+      <c r="B48" s="8" t="n">
         <v>0.73</v>
       </c>
-      <c r="C48" s="10" t="n">
+      <c r="C48" s="8" t="n">
         <f aca="false">1-B48</f>
         <v>0.27</v>
       </c>
@@ -25430,17 +25412,17 @@
         <f aca="false">B48*B$3 + C48*C$3</f>
         <v>0.00705048421589691</v>
       </c>
-      <c r="F48" s="12" t="n">
+      <c r="F48" s="11" t="n">
         <f aca="false">E48/D48</f>
         <v>0.198522413319183</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="10" t="n">
+      <c r="B49" s="8" t="n">
         <f aca="false">B47+0.02</f>
         <v>0.74</v>
       </c>
-      <c r="C49" s="10" t="n">
+      <c r="C49" s="8" t="n">
         <f aca="false">1-B49</f>
         <v>0.26</v>
       </c>
@@ -25452,17 +25434,17 @@
         <f aca="false">B49*B$3 + C49*C$3</f>
         <v>0.00703596325963047</v>
       </c>
-      <c r="F49" s="12" t="n">
+      <c r="F49" s="11" t="n">
         <f aca="false">E49/D49</f>
         <v>0.198394730012048</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="10" t="n">
+      <c r="B50" s="8" t="n">
         <f aca="false">B49+0.02</f>
         <v>0.76</v>
       </c>
-      <c r="C50" s="10" t="n">
+      <c r="C50" s="8" t="n">
         <f aca="false">1-B50</f>
         <v>0.24</v>
       </c>
@@ -25474,17 +25456,17 @@
         <f aca="false">B50*B$3 + C50*C$3</f>
         <v>0.00700692134709759</v>
       </c>
-      <c r="F50" s="12" t="n">
+      <c r="F50" s="11" t="n">
         <f aca="false">E50/D50</f>
         <v>0.197949341081221</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="10" t="n">
+      <c r="B51" s="8" t="n">
         <f aca="false">B50+0.02</f>
         <v>0.78</v>
       </c>
-      <c r="C51" s="10" t="n">
+      <c r="C51" s="8" t="n">
         <f aca="false">1-B51</f>
         <v>0.22</v>
       </c>
@@ -25496,17 +25478,17 @@
         <f aca="false">B51*B$3 + C51*C$3</f>
         <v>0.0069778794345647</v>
       </c>
-      <c r="F51" s="12" t="n">
+      <c r="F51" s="11" t="n">
         <f aca="false">E51/D51</f>
         <v>0.197249921910797</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="10" t="n">
+      <c r="B52" s="8" t="n">
         <f aca="false">B51+0.02</f>
         <v>0.8</v>
       </c>
-      <c r="C52" s="10" t="n">
+      <c r="C52" s="8" t="n">
         <f aca="false">1-B52</f>
         <v>0.2</v>
       </c>
@@ -25518,17 +25500,17 @@
         <f aca="false">B52*B$3 + C52*C$3</f>
         <v>0.00694883752203182</v>
       </c>
-      <c r="F52" s="12" t="n">
+      <c r="F52" s="11" t="n">
         <f aca="false">E52/D52</f>
         <v>0.196298222674184</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="10" t="n">
+      <c r="B53" s="8" t="n">
         <f aca="false">B52+0.02</f>
         <v>0.82</v>
       </c>
-      <c r="C53" s="10" t="n">
+      <c r="C53" s="8" t="n">
         <f aca="false">1-B53</f>
         <v>0.18</v>
       </c>
@@ -25540,17 +25522,17 @@
         <f aca="false">B53*B$3 + C53*C$3</f>
         <v>0.00691979560949893</v>
       </c>
-      <c r="F53" s="12" t="n">
+      <c r="F53" s="11" t="n">
         <f aca="false">E53/D53</f>
         <v>0.195098887635855</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="10" t="n">
+      <c r="B54" s="8" t="n">
         <f aca="false">B53+0.02</f>
         <v>0.84</v>
       </c>
-      <c r="C54" s="10" t="n">
+      <c r="C54" s="8" t="n">
         <f aca="false">1-B54</f>
         <v>0.16</v>
       </c>
@@ -25562,17 +25544,17 @@
         <f aca="false">B54*B$3 + C54*C$3</f>
         <v>0.00689075369696605</v>
       </c>
-      <c r="F54" s="12" t="n">
+      <c r="F54" s="11" t="n">
         <f aca="false">E54/D54</f>
         <v>0.193659347781608</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="10" t="n">
+      <c r="B55" s="8" t="n">
         <f aca="false">B54+0.02</f>
         <v>0.86</v>
       </c>
-      <c r="C55" s="10" t="n">
+      <c r="C55" s="8" t="n">
         <f aca="false">1-B55</f>
         <v>0.14</v>
       </c>
@@ -25584,17 +25566,17 @@
         <f aca="false">B55*B$3 + C55*C$3</f>
         <v>0.00686171178443316</v>
       </c>
-      <c r="F55" s="12" t="n">
+      <c r="F55" s="11" t="n">
         <f aca="false">E55/D55</f>
         <v>0.19198962733272</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="10" t="n">
+      <c r="B56" s="8" t="n">
         <f aca="false">B55+0.02</f>
         <v>0.88</v>
       </c>
-      <c r="C56" s="10" t="n">
+      <c r="C56" s="8" t="n">
         <f aca="false">1-B56</f>
         <v>0.12</v>
       </c>
@@ -25606,17 +25588,17 @@
         <f aca="false">B56*B$3 + C56*C$3</f>
         <v>0.00683266987190028</v>
       </c>
-      <c r="F56" s="12" t="n">
+      <c r="F56" s="11" t="n">
         <f aca="false">E56/D56</f>
         <v>0.190102074848599</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="10" t="n">
+      <c r="B57" s="8" t="n">
         <f aca="false">B56+0.02</f>
         <v>0.9</v>
       </c>
-      <c r="C57" s="10" t="n">
+      <c r="C57" s="8" t="n">
         <f aca="false">1-B57</f>
         <v>0.0999999999999995</v>
       </c>
@@ -25628,17 +25610,17 @@
         <f aca="false">B57*B$3 + C57*C$3</f>
         <v>0.00680362795936739</v>
       </c>
-      <c r="F57" s="12" t="n">
+      <c r="F57" s="11" t="n">
         <f aca="false">E57/D57</f>
         <v>0.188011033765084</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="10" t="n">
+      <c r="B58" s="8" t="n">
         <f aca="false">B57+0.02</f>
         <v>0.92</v>
       </c>
-      <c r="C58" s="10" t="n">
+      <c r="C58" s="8" t="n">
         <f aca="false">1-B58</f>
         <v>0.0799999999999995</v>
       </c>
@@ -25650,17 +25632,17 @@
         <f aca="false">B58*B$3 + C58*C$3</f>
         <v>0.00677458604683451</v>
       </c>
-      <c r="F58" s="12" t="n">
+      <c r="F58" s="11" t="n">
         <f aca="false">E58/D58</f>
         <v>0.185732469997929</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="10" t="n">
+      <c r="B59" s="8" t="n">
         <f aca="false">B58+0.02</f>
         <v>0.94</v>
       </c>
-      <c r="C59" s="10" t="n">
+      <c r="C59" s="8" t="n">
         <f aca="false">1-B59</f>
         <v>0.0599999999999995</v>
       </c>
@@ -25672,17 +25654,17 @@
         <f aca="false">B59*B$3 + C59*C$3</f>
         <v>0.00674554413430162</v>
       </c>
-      <c r="F59" s="12" t="n">
+      <c r="F59" s="11" t="n">
         <f aca="false">E59/D59</f>
         <v>0.183283575487641</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="10" t="n">
+      <c r="B60" s="8" t="n">
         <f aca="false">B59+0.02</f>
         <v>0.960000000000001</v>
       </c>
-      <c r="C60" s="10" t="n">
+      <c r="C60" s="8" t="n">
         <f aca="false">1-B60</f>
         <v>0.0399999999999995</v>
       </c>
@@ -25694,17 +25676,17 @@
         <f aca="false">B60*B$3 + C60*C$3</f>
         <v>0.00671650222176874</v>
       </c>
-      <c r="F60" s="12" t="n">
+      <c r="F60" s="11" t="n">
         <f aca="false">E60/D60</f>
         <v>0.180682366291003</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="10" t="n">
+      <c r="B61" s="8" t="n">
         <f aca="false">B60+0.02</f>
         <v>0.98</v>
       </c>
-      <c r="C61" s="10" t="n">
+      <c r="C61" s="8" t="n">
         <f aca="false">1-B61</f>
         <v>0.0199999999999995</v>
       </c>
@@ -25716,17 +25698,17 @@
         <f aca="false">B61*B$3 + C61*C$3</f>
         <v>0.00668746030923585</v>
       </c>
-      <c r="F61" s="12" t="n">
+      <c r="F61" s="11" t="n">
         <f aca="false">E61/D61</f>
         <v>0.17794729222556</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="10" t="n">
+      <c r="B62" s="8" t="n">
         <f aca="false">B61+0.02</f>
         <v>1</v>
       </c>
-      <c r="C62" s="10" t="n">
+      <c r="C62" s="8" t="n">
         <f aca="false">1-B62</f>
         <v>0</v>
       </c>
@@ -25738,7 +25720,7 @@
         <f aca="false">B62*B$3 + C62*C$3</f>
         <v>0.00665841839670297</v>
       </c>
-      <c r="F62" s="12" t="n">
+      <c r="F62" s="11" t="n">
         <f aca="false">E62/D62</f>
         <v>0.175096872458789</v>
       </c>
@@ -25755,13 +25737,13 @@
       <c r="C67" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="10" t="s">
+      <c r="D67" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="E67" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F67" s="11" t="s">
+      <c r="F67" s="10" t="s">
         <v>17</v>
       </c>
       <c r="G67" s="0" t="s">
@@ -25769,1328 +25751,1328 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C68" s="10" t="n">
+      <c r="B68" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C68" s="8" t="n">
         <f aca="false">1-B68</f>
         <v>1</v>
       </c>
-      <c r="D68" s="10" t="n">
-        <f aca="false">B68*D$48</f>
-        <v>0</v>
-      </c>
-      <c r="E68" s="10" t="n">
-        <f aca="false">B68*E$48</f>
-        <v>0</v>
-      </c>
-      <c r="F68" s="11" t="e">
+      <c r="D68" s="8" t="n">
+        <f aca="false">B68*D$47</f>
+        <v>0</v>
+      </c>
+      <c r="E68" s="8" t="n">
+        <f aca="false">B68*E$47</f>
+        <v>0</v>
+      </c>
+      <c r="F68" s="10" t="e">
         <f aca="false">E68/D68</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G68" s="16" t="n">
+      <c r="G68" s="14" t="n">
         <f aca="false">E68-0.5*8*D68^2</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="10" t="n">
+      <c r="B69" s="8" t="n">
         <f aca="false">B68+0.02</f>
         <v>0.02</v>
       </c>
-      <c r="C69" s="10" t="n">
+      <c r="C69" s="8" t="n">
         <f aca="false">1-B69</f>
         <v>0.98</v>
       </c>
-      <c r="D69" s="10" t="n">
-        <f aca="false">B69*D$48</f>
-        <v>0.000710296041441044</v>
-      </c>
-      <c r="E69" s="10" t="n">
-        <f aca="false">B69*E$48</f>
-        <v>0.000141009684317938</v>
-      </c>
-      <c r="F69" s="11" t="n">
+      <c r="D69" s="8" t="n">
+        <f aca="false">B69*D$47</f>
+        <v>0.0007115265690196</v>
+      </c>
+      <c r="E69" s="8" t="n">
+        <f aca="false">B69*E$47</f>
+        <v>0.000141300103443267</v>
+      </c>
+      <c r="F69" s="10" t="n">
         <f aca="false">E69/D69</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G69" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G69" s="14" t="n">
         <f aca="false">E69-0.5*8*D69^2</f>
-        <v>0.000138991602451991</v>
+        <v>0.000139275023209584</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="10" t="n">
+      <c r="B70" s="8" t="n">
         <f aca="false">B69+0.02</f>
         <v>0.04</v>
       </c>
-      <c r="C70" s="10" t="n">
+      <c r="C70" s="8" t="n">
         <f aca="false">1-B70</f>
         <v>0.96</v>
       </c>
-      <c r="D70" s="10" t="n">
-        <f aca="false">B70*D$48</f>
-        <v>0.00142059208288209</v>
-      </c>
-      <c r="E70" s="10" t="n">
-        <f aca="false">B70*E$48</f>
-        <v>0.000282019368635876</v>
-      </c>
-      <c r="F70" s="11" t="n">
+      <c r="D70" s="8" t="n">
+        <f aca="false">B70*D$47</f>
+        <v>0.0014230531380392</v>
+      </c>
+      <c r="E70" s="8" t="n">
+        <f aca="false">B70*E$47</f>
+        <v>0.000282600206886534</v>
+      </c>
+      <c r="F70" s="10" t="n">
         <f aca="false">E70/D70</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G70" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G70" s="14" t="n">
         <f aca="false">E70-0.5*8*D70^2</f>
-        <v>0.000273947041172087</v>
+        <v>0.000274499885951802</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="10" t="n">
+      <c r="B71" s="8" t="n">
         <f aca="false">B70+0.02</f>
         <v>0.06</v>
       </c>
-      <c r="C71" s="10" t="n">
+      <c r="C71" s="8" t="n">
         <f aca="false">1-B71</f>
         <v>0.94</v>
       </c>
-      <c r="D71" s="10" t="n">
-        <f aca="false">B71*D$48</f>
-        <v>0.00213088812432313</v>
-      </c>
-      <c r="E71" s="10" t="n">
-        <f aca="false">B71*E$48</f>
-        <v>0.000423029052953815</v>
-      </c>
-      <c r="F71" s="11" t="n">
+      <c r="D71" s="8" t="n">
+        <f aca="false">B71*D$47</f>
+        <v>0.0021345797070588</v>
+      </c>
+      <c r="E71" s="8" t="n">
+        <f aca="false">B71*E$47</f>
+        <v>0.000423900310329802</v>
+      </c>
+      <c r="F71" s="10" t="n">
         <f aca="false">E71/D71</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G71" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G71" s="14" t="n">
         <f aca="false">E71-0.5*8*D71^2</f>
-        <v>0.000404866316160289</v>
+        <v>0.000405674588226653</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="10" t="n">
+      <c r="B72" s="8" t="n">
         <f aca="false">B71+0.02</f>
         <v>0.08</v>
       </c>
-      <c r="C72" s="10" t="n">
+      <c r="C72" s="8" t="n">
         <f aca="false">1-B72</f>
         <v>0.92</v>
       </c>
-      <c r="D72" s="10" t="n">
-        <f aca="false">B72*D$48</f>
-        <v>0.00284118416576417</v>
-      </c>
-      <c r="E72" s="10" t="n">
-        <f aca="false">B72*E$48</f>
-        <v>0.000564038737271753</v>
-      </c>
-      <c r="F72" s="11" t="n">
+      <c r="D72" s="8" t="n">
+        <f aca="false">B72*D$47</f>
+        <v>0.0028461062760784</v>
+      </c>
+      <c r="E72" s="8" t="n">
+        <f aca="false">B72*E$47</f>
+        <v>0.000565200413773069</v>
+      </c>
+      <c r="F72" s="10" t="n">
         <f aca="false">E72/D72</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G72" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G72" s="14" t="n">
         <f aca="false">E72-0.5*8*D72^2</f>
-        <v>0.000531749427416597</v>
+        <v>0.000532799130034137</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="10" t="n">
+      <c r="B73" s="8" t="n">
         <f aca="false">B72+0.02</f>
         <v>0.1</v>
       </c>
-      <c r="C73" s="10" t="n">
+      <c r="C73" s="8" t="n">
         <f aca="false">1-B73</f>
         <v>0.9</v>
       </c>
-      <c r="D73" s="10" t="n">
-        <f aca="false">B73*D$48</f>
-        <v>0.00355148020720522</v>
-      </c>
-      <c r="E73" s="10" t="n">
-        <f aca="false">B73*E$48</f>
-        <v>0.000705048421589691</v>
-      </c>
-      <c r="F73" s="11" t="n">
+      <c r="D73" s="8" t="n">
+        <f aca="false">B73*D$47</f>
+        <v>0.003557632845098</v>
+      </c>
+      <c r="E73" s="8" t="n">
+        <f aca="false">B73*E$47</f>
+        <v>0.000706500517216336</v>
+      </c>
+      <c r="F73" s="10" t="n">
         <f aca="false">E73/D73</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G73" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G73" s="14" t="n">
         <f aca="false">E73-0.5*8*D73^2</f>
-        <v>0.00065459637494101</v>
+        <v>0.000655873511374256</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="10" t="n">
+      <c r="B74" s="8" t="n">
         <f aca="false">B73+0.02</f>
         <v>0.12</v>
       </c>
-      <c r="C74" s="10" t="n">
+      <c r="C74" s="8" t="n">
         <f aca="false">1-B74</f>
         <v>0.88</v>
       </c>
-      <c r="D74" s="10" t="n">
-        <f aca="false">B74*D$48</f>
-        <v>0.00426177624864626</v>
-      </c>
-      <c r="E74" s="10" t="n">
-        <f aca="false">B74*E$48</f>
-        <v>0.00084605810590763</v>
-      </c>
-      <c r="F74" s="11" t="n">
+      <c r="D74" s="8" t="n">
+        <f aca="false">B74*D$47</f>
+        <v>0.0042691594141176</v>
+      </c>
+      <c r="E74" s="8" t="n">
+        <f aca="false">B74*E$47</f>
+        <v>0.000847800620659603</v>
+      </c>
+      <c r="F74" s="10" t="n">
         <f aca="false">E74/D74</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G74" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G74" s="14" t="n">
         <f aca="false">E74-0.5*8*D74^2</f>
-        <v>0.000773407158733528</v>
+        <v>0.000774897732247007</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="10" t="n">
+      <c r="B75" s="8" t="n">
         <f aca="false">B74+0.02</f>
         <v>0.14</v>
       </c>
-      <c r="C75" s="10" t="n">
+      <c r="C75" s="8" t="n">
         <f aca="false">1-B75</f>
         <v>0.86</v>
       </c>
-      <c r="D75" s="10" t="n">
-        <f aca="false">B75*D$48</f>
-        <v>0.00497207229008731</v>
-      </c>
-      <c r="E75" s="10" t="n">
-        <f aca="false">B75*E$48</f>
-        <v>0.000987067790225568</v>
-      </c>
-      <c r="F75" s="11" t="n">
+      <c r="D75" s="8" t="n">
+        <f aca="false">B75*D$47</f>
+        <v>0.0049806859831372</v>
+      </c>
+      <c r="E75" s="8" t="n">
+        <f aca="false">B75*E$47</f>
+        <v>0.00098910072410287</v>
+      </c>
+      <c r="F75" s="10" t="n">
         <f aca="false">E75/D75</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G75" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G75" s="14" t="n">
         <f aca="false">E75-0.5*8*D75^2</f>
-        <v>0.000888181778794152</v>
+        <v>0.000889871792652393</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="10" t="n">
+      <c r="B76" s="8" t="n">
         <f aca="false">B75+0.02</f>
         <v>0.16</v>
       </c>
-      <c r="C76" s="10" t="n">
+      <c r="C76" s="8" t="n">
         <f aca="false">1-B76</f>
         <v>0.84</v>
       </c>
-      <c r="D76" s="10" t="n">
-        <f aca="false">B76*D$48</f>
-        <v>0.00568236833152835</v>
-      </c>
-      <c r="E76" s="10" t="n">
-        <f aca="false">B76*E$48</f>
-        <v>0.00112807747454351</v>
-      </c>
-      <c r="F76" s="11" t="n">
+      <c r="D76" s="8" t="n">
+        <f aca="false">B76*D$47</f>
+        <v>0.0056922125521568</v>
+      </c>
+      <c r="E76" s="8" t="n">
+        <f aca="false">B76*E$47</f>
+        <v>0.00113040082754614</v>
+      </c>
+      <c r="F76" s="10" t="n">
         <f aca="false">E76/D76</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G76" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G76" s="14" t="n">
         <f aca="false">E76-0.5*8*D76^2</f>
-        <v>0.000998920235122881</v>
+        <v>0.00100079569259041</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="10" t="n">
+      <c r="B77" s="8" t="n">
         <f aca="false">B76+0.02</f>
         <v>0.18</v>
       </c>
-      <c r="C77" s="10" t="n">
+      <c r="C77" s="8" t="n">
         <f aca="false">1-B77</f>
         <v>0.82</v>
       </c>
-      <c r="D77" s="10" t="n">
-        <f aca="false">B77*D$48</f>
-        <v>0.00639266437296939</v>
-      </c>
-      <c r="E77" s="10" t="n">
-        <f aca="false">B77*E$48</f>
-        <v>0.00126908715886144</v>
-      </c>
-      <c r="F77" s="11" t="n">
+      <c r="D77" s="8" t="n">
+        <f aca="false">B77*D$47</f>
+        <v>0.0064037391211764</v>
+      </c>
+      <c r="E77" s="8" t="n">
+        <f aca="false">B77*E$47</f>
+        <v>0.0012717009309894</v>
+      </c>
+      <c r="F77" s="10" t="n">
         <f aca="false">E77/D77</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G77" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G77" s="14" t="n">
         <f aca="false">E77-0.5*8*D77^2</f>
-        <v>0.00110562252771972</v>
+        <v>0.00110766943206106</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="10" t="n">
+      <c r="B78" s="8" t="n">
         <f aca="false">B77+0.02</f>
         <v>0.2</v>
       </c>
-      <c r="C78" s="10" t="n">
+      <c r="C78" s="8" t="n">
         <f aca="false">1-B78</f>
         <v>0.8</v>
       </c>
-      <c r="D78" s="10" t="n">
-        <f aca="false">B78*D$48</f>
-        <v>0.00710296041441044</v>
-      </c>
-      <c r="E78" s="10" t="n">
-        <f aca="false">B78*E$48</f>
-        <v>0.00141009684317938</v>
-      </c>
-      <c r="F78" s="11" t="n">
+      <c r="D78" s="8" t="n">
+        <f aca="false">B78*D$47</f>
+        <v>0.007115265690196</v>
+      </c>
+      <c r="E78" s="8" t="n">
+        <f aca="false">B78*E$47</f>
+        <v>0.00141300103443267</v>
+      </c>
+      <c r="F78" s="10" t="n">
         <f aca="false">E78/D78</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G78" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G78" s="14" t="n">
         <f aca="false">E78-0.5*8*D78^2</f>
-        <v>0.00120828865658466</v>
+        <v>0.00121049301106435</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="10" t="n">
+      <c r="B79" s="8" t="n">
         <f aca="false">B78+0.02</f>
         <v>0.22</v>
       </c>
-      <c r="C79" s="10" t="n">
+      <c r="C79" s="8" t="n">
         <f aca="false">1-B79</f>
         <v>0.78</v>
       </c>
-      <c r="D79" s="10" t="n">
-        <f aca="false">B79*D$48</f>
-        <v>0.00781325645585148</v>
-      </c>
-      <c r="E79" s="10" t="n">
-        <f aca="false">B79*E$48</f>
-        <v>0.00155110652749732</v>
-      </c>
-      <c r="F79" s="11" t="n">
+      <c r="D79" s="8" t="n">
+        <f aca="false">B79*D$47</f>
+        <v>0.0078267922592156</v>
+      </c>
+      <c r="E79" s="8" t="n">
+        <f aca="false">B79*E$47</f>
+        <v>0.00155430113787594</v>
+      </c>
+      <c r="F79" s="10" t="n">
         <f aca="false">E79/D79</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G79" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G79" s="14" t="n">
         <f aca="false">E79-0.5*8*D79^2</f>
-        <v>0.0013069186217177</v>
+        <v>0.00130926642960027</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="10" t="n">
+      <c r="B80" s="8" t="n">
         <f aca="false">B79+0.02</f>
         <v>0.24</v>
       </c>
-      <c r="C80" s="10" t="n">
+      <c r="C80" s="8" t="n">
         <f aca="false">1-B80</f>
         <v>0.76</v>
       </c>
-      <c r="D80" s="10" t="n">
-        <f aca="false">B80*D$48</f>
-        <v>0.00852355249729252</v>
-      </c>
-      <c r="E80" s="10" t="n">
-        <f aca="false">B80*E$48</f>
-        <v>0.00169211621181526</v>
-      </c>
-      <c r="F80" s="11" t="n">
+      <c r="D80" s="8" t="n">
+        <f aca="false">B80*D$47</f>
+        <v>0.0085383188282352</v>
+      </c>
+      <c r="E80" s="8" t="n">
+        <f aca="false">B80*E$47</f>
+        <v>0.00169560124131921</v>
+      </c>
+      <c r="F80" s="10" t="n">
         <f aca="false">E80/D80</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G80" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G80" s="14" t="n">
         <f aca="false">E80-0.5*8*D80^2</f>
-        <v>0.00140151242311885</v>
+        <v>0.00140398968766882</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="10" t="n">
+      <c r="B81" s="8" t="n">
         <f aca="false">B80+0.02</f>
         <v>0.26</v>
       </c>
-      <c r="C81" s="10" t="n">
+      <c r="C81" s="8" t="n">
         <f aca="false">1-B81</f>
         <v>0.74</v>
       </c>
-      <c r="D81" s="10" t="n">
-        <f aca="false">B81*D$48</f>
-        <v>0.00923384853873357</v>
-      </c>
-      <c r="E81" s="10" t="n">
-        <f aca="false">B81*E$48</f>
-        <v>0.0018331258961332</v>
-      </c>
-      <c r="F81" s="11" t="n">
+      <c r="D81" s="8" t="n">
+        <f aca="false">B81*D$47</f>
+        <v>0.0092498453972548</v>
+      </c>
+      <c r="E81" s="8" t="n">
+        <f aca="false">B81*E$47</f>
+        <v>0.00183690134476247</v>
+      </c>
+      <c r="F81" s="10" t="n">
         <f aca="false">E81/D81</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G81" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G81" s="14" t="n">
         <f aca="false">E81-0.5*8*D81^2</f>
-        <v>0.00149207006078811</v>
+        <v>0.00149466278527001</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="10" t="n">
+      <c r="B82" s="8" t="n">
         <f aca="false">B81+0.02</f>
         <v>0.28</v>
       </c>
-      <c r="C82" s="10" t="n">
+      <c r="C82" s="8" t="n">
         <f aca="false">1-B82</f>
         <v>0.72</v>
       </c>
-      <c r="D82" s="10" t="n">
-        <f aca="false">B82*D$48</f>
-        <v>0.00994414458017461</v>
-      </c>
-      <c r="E82" s="10" t="n">
-        <f aca="false">B82*E$48</f>
-        <v>0.00197413558045114</v>
-      </c>
-      <c r="F82" s="11" t="n">
+      <c r="D82" s="8" t="n">
+        <f aca="false">B82*D$47</f>
+        <v>0.0099613719662744</v>
+      </c>
+      <c r="E82" s="8" t="n">
+        <f aca="false">B82*E$47</f>
+        <v>0.00197820144820574</v>
+      </c>
+      <c r="F82" s="10" t="n">
         <f aca="false">E82/D82</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G82" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G82" s="14" t="n">
         <f aca="false">E82-0.5*8*D82^2</f>
-        <v>0.00157859153472547</v>
+        <v>0.00158128572240383</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="10" t="n">
+      <c r="B83" s="8" t="n">
         <f aca="false">B82+0.02</f>
         <v>0.3</v>
       </c>
-      <c r="C83" s="10" t="n">
+      <c r="C83" s="8" t="n">
         <f aca="false">1-B83</f>
         <v>0.7</v>
       </c>
-      <c r="D83" s="10" t="n">
-        <f aca="false">B83*D$48</f>
-        <v>0.0106544406216157</v>
-      </c>
-      <c r="E83" s="10" t="n">
-        <f aca="false">B83*E$48</f>
-        <v>0.00211514526476907</v>
-      </c>
-      <c r="F83" s="11" t="n">
+      <c r="D83" s="8" t="n">
+        <f aca="false">B83*D$47</f>
+        <v>0.010672898535294</v>
+      </c>
+      <c r="E83" s="8" t="n">
+        <f aca="false">B83*E$47</f>
+        <v>0.00211950155164901</v>
+      </c>
+      <c r="F83" s="10" t="n">
         <f aca="false">E83/D83</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G83" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G83" s="14" t="n">
         <f aca="false">E83-0.5*8*D83^2</f>
-        <v>0.00166107684493094</v>
+        <v>0.00166385849907028</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="10" t="n">
+      <c r="B84" s="8" t="n">
         <f aca="false">B83+0.02</f>
         <v>0.32</v>
       </c>
-      <c r="C84" s="10" t="n">
+      <c r="C84" s="8" t="n">
         <f aca="false">1-B84</f>
         <v>0.68</v>
       </c>
-      <c r="D84" s="10" t="n">
-        <f aca="false">B84*D$48</f>
-        <v>0.0113647366630567</v>
-      </c>
-      <c r="E84" s="10" t="n">
-        <f aca="false">B84*E$48</f>
-        <v>0.00225615494908701</v>
-      </c>
-      <c r="F84" s="11" t="n">
+      <c r="D84" s="8" t="n">
+        <f aca="false">B84*D$47</f>
+        <v>0.0113844251043136</v>
+      </c>
+      <c r="E84" s="8" t="n">
+        <f aca="false">B84*E$47</f>
+        <v>0.00226080165509228</v>
+      </c>
+      <c r="F84" s="10" t="n">
         <f aca="false">E84/D84</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G84" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G84" s="14" t="n">
         <f aca="false">E84-0.5*8*D84^2</f>
-        <v>0.00173952599140451</v>
+        <v>0.00174238111526937</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="10" t="n">
+      <c r="B85" s="8" t="n">
         <f aca="false">B84+0.02</f>
         <v>0.34</v>
       </c>
-      <c r="C85" s="10" t="n">
+      <c r="C85" s="8" t="n">
         <f aca="false">1-B85</f>
         <v>0.66</v>
       </c>
-      <c r="D85" s="10" t="n">
-        <f aca="false">B85*D$48</f>
-        <v>0.0120750327044977</v>
-      </c>
-      <c r="E85" s="10" t="n">
-        <f aca="false">B85*E$48</f>
-        <v>0.00239716463340495</v>
-      </c>
-      <c r="F85" s="11" t="n">
+      <c r="D85" s="8" t="n">
+        <f aca="false">B85*D$47</f>
+        <v>0.0120959516733332</v>
+      </c>
+      <c r="E85" s="8" t="n">
+        <f aca="false">B85*E$47</f>
+        <v>0.00240210175853554</v>
+      </c>
+      <c r="F85" s="10" t="n">
         <f aca="false">E85/D85</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G85" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G85" s="14" t="n">
         <f aca="false">E85-0.5*8*D85^2</f>
-        <v>0.00181393897414619</v>
+        <v>0.00181685357100109</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="10" t="n">
+      <c r="B86" s="8" t="n">
         <f aca="false">B85+0.02</f>
         <v>0.36</v>
       </c>
-      <c r="C86" s="10" t="n">
+      <c r="C86" s="8" t="n">
         <f aca="false">1-B86</f>
         <v>0.64</v>
       </c>
-      <c r="D86" s="10" t="n">
-        <f aca="false">B86*D$48</f>
-        <v>0.0127853287459388</v>
-      </c>
-      <c r="E86" s="10" t="n">
-        <f aca="false">B86*E$48</f>
-        <v>0.00253817431772289</v>
-      </c>
-      <c r="F86" s="11" t="n">
+      <c r="D86" s="8" t="n">
+        <f aca="false">B86*D$47</f>
+        <v>0.0128074782423528</v>
+      </c>
+      <c r="E86" s="8" t="n">
+        <f aca="false">B86*E$47</f>
+        <v>0.00254340186197881</v>
+      </c>
+      <c r="F86" s="10" t="n">
         <f aca="false">E86/D86</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G86" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G86" s="14" t="n">
         <f aca="false">E86-0.5*8*D86^2</f>
-        <v>0.00188431579315597</v>
+        <v>0.00188727586626545</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="10" t="n">
+      <c r="B87" s="8" t="n">
         <f aca="false">B86+0.02</f>
         <v>0.38</v>
       </c>
-      <c r="C87" s="10" t="n">
+      <c r="C87" s="8" t="n">
         <f aca="false">1-B87</f>
         <v>0.62</v>
       </c>
-      <c r="D87" s="10" t="n">
-        <f aca="false">B87*D$48</f>
-        <v>0.0134956247873798</v>
-      </c>
-      <c r="E87" s="10" t="n">
-        <f aca="false">B87*E$48</f>
-        <v>0.00267918400204083</v>
-      </c>
-      <c r="F87" s="11" t="n">
+      <c r="D87" s="8" t="n">
+        <f aca="false">B87*D$47</f>
+        <v>0.0135190048113724</v>
+      </c>
+      <c r="E87" s="8" t="n">
+        <f aca="false">B87*E$47</f>
+        <v>0.00268470196542208</v>
+      </c>
+      <c r="F87" s="10" t="n">
         <f aca="false">E87/D87</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G87" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G87" s="14" t="n">
         <f aca="false">E87-0.5*8*D87^2</f>
-        <v>0.00195065644843386</v>
+        <v>0.00195364800106244</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="10" t="n">
+      <c r="B88" s="8" t="n">
         <f aca="false">B87+0.02</f>
         <v>0.4</v>
       </c>
-      <c r="C88" s="10" t="n">
+      <c r="C88" s="8" t="n">
         <f aca="false">1-B88</f>
         <v>0.6</v>
       </c>
-      <c r="D88" s="10" t="n">
-        <f aca="false">B88*D$48</f>
-        <v>0.0142059208288209</v>
-      </c>
-      <c r="E88" s="10" t="n">
-        <f aca="false">B88*E$48</f>
-        <v>0.00282019368635877</v>
-      </c>
-      <c r="F88" s="11" t="n">
+      <c r="D88" s="8" t="n">
+        <f aca="false">B88*D$47</f>
+        <v>0.014230531380392</v>
+      </c>
+      <c r="E88" s="8" t="n">
+        <f aca="false">B88*E$47</f>
+        <v>0.00282600206886534</v>
+      </c>
+      <c r="F88" s="10" t="n">
         <f aca="false">E88/D88</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G88" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G88" s="14" t="n">
         <f aca="false">E88-0.5*8*D88^2</f>
-        <v>0.00201296093997986</v>
+        <v>0.00201596997539206</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="10" t="n">
+      <c r="B89" s="8" t="n">
         <f aca="false">B88+0.02</f>
         <v>0.42</v>
       </c>
-      <c r="C89" s="10" t="n">
+      <c r="C89" s="8" t="n">
         <f aca="false">1-B89</f>
         <v>0.58</v>
       </c>
-      <c r="D89" s="10" t="n">
-        <f aca="false">B89*D$48</f>
-        <v>0.0149162168702619</v>
-      </c>
-      <c r="E89" s="10" t="n">
-        <f aca="false">B89*E$48</f>
-        <v>0.0029612033706767</v>
-      </c>
-      <c r="F89" s="11" t="n">
+      <c r="D89" s="8" t="n">
+        <f aca="false">B89*D$47</f>
+        <v>0.0149420579494116</v>
+      </c>
+      <c r="E89" s="8" t="n">
+        <f aca="false">B89*E$47</f>
+        <v>0.00296730217230861</v>
+      </c>
+      <c r="F89" s="10" t="n">
         <f aca="false">E89/D89</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G89" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G89" s="14" t="n">
         <f aca="false">E89-0.5*8*D89^2</f>
-        <v>0.00207122926779396</v>
+        <v>0.00207424178925431</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="10" t="n">
+      <c r="B90" s="8" t="n">
         <f aca="false">B89+0.02</f>
         <v>0.44</v>
       </c>
-      <c r="C90" s="10" t="n">
+      <c r="C90" s="8" t="n">
         <f aca="false">1-B90</f>
         <v>0.56</v>
       </c>
-      <c r="D90" s="10" t="n">
-        <f aca="false">B90*D$48</f>
-        <v>0.015626512911703</v>
-      </c>
-      <c r="E90" s="10" t="n">
-        <f aca="false">B90*E$48</f>
-        <v>0.00310221305499464</v>
-      </c>
-      <c r="F90" s="11" t="n">
+      <c r="D90" s="8" t="n">
+        <f aca="false">B90*D$47</f>
+        <v>0.0156535845184312</v>
+      </c>
+      <c r="E90" s="8" t="n">
+        <f aca="false">B90*E$47</f>
+        <v>0.00310860227575188</v>
+      </c>
+      <c r="F90" s="10" t="n">
         <f aca="false">E90/D90</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G90" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G90" s="14" t="n">
         <f aca="false">E90-0.5*8*D90^2</f>
-        <v>0.00212546143187616</v>
+        <v>0.0021284634426492</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="10" t="n">
+      <c r="B91" s="8" t="n">
         <f aca="false">B90+0.02</f>
         <v>0.46</v>
       </c>
-      <c r="C91" s="10" t="n">
+      <c r="C91" s="8" t="n">
         <f aca="false">1-B91</f>
         <v>0.54</v>
       </c>
-      <c r="D91" s="10" t="n">
-        <f aca="false">B91*D$48</f>
-        <v>0.016336808953144</v>
-      </c>
-      <c r="E91" s="10" t="n">
-        <f aca="false">B91*E$48</f>
-        <v>0.00324322273931258</v>
-      </c>
-      <c r="F91" s="11" t="n">
+      <c r="D91" s="8" t="n">
+        <f aca="false">B91*D$47</f>
+        <v>0.0163651110874508</v>
+      </c>
+      <c r="E91" s="8" t="n">
+        <f aca="false">B91*E$47</f>
+        <v>0.00324990237919515</v>
+      </c>
+      <c r="F91" s="10" t="n">
         <f aca="false">E91/D91</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G91" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G91" s="14" t="n">
         <f aca="false">E91-0.5*8*D91^2</f>
-        <v>0.00217565743222648</v>
+        <v>0.00217863493557673</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="10" t="n">
+      <c r="B92" s="8" t="n">
         <f aca="false">B91+0.02</f>
         <v>0.48</v>
       </c>
-      <c r="C92" s="10" t="n">
+      <c r="C92" s="8" t="n">
         <f aca="false">1-B92</f>
         <v>0.52</v>
       </c>
-      <c r="D92" s="10" t="n">
-        <f aca="false">B92*D$48</f>
-        <v>0.0170471049945851</v>
-      </c>
-      <c r="E92" s="10" t="n">
-        <f aca="false">B92*E$48</f>
-        <v>0.00338423242363052</v>
-      </c>
-      <c r="F92" s="11" t="n">
+      <c r="D92" s="8" t="n">
+        <f aca="false">B92*D$47</f>
+        <v>0.0170766376564704</v>
+      </c>
+      <c r="E92" s="8" t="n">
+        <f aca="false">B92*E$47</f>
+        <v>0.00339120248263841</v>
+      </c>
+      <c r="F92" s="10" t="n">
         <f aca="false">E92/D92</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G92" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G92" s="14" t="n">
         <f aca="false">E92-0.5*8*D92^2</f>
-        <v>0.00222181726884489</v>
+        <v>0.00222475626803688</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="10" t="n">
+      <c r="B93" s="8" t="n">
         <f aca="false">B92+0.02</f>
         <v>0.5</v>
       </c>
-      <c r="C93" s="10" t="n">
+      <c r="C93" s="8" t="n">
         <f aca="false">1-B93</f>
         <v>0.5</v>
       </c>
-      <c r="D93" s="10" t="n">
-        <f aca="false">B93*D$48</f>
-        <v>0.0177574010360261</v>
-      </c>
-      <c r="E93" s="10" t="n">
-        <f aca="false">B93*E$48</f>
-        <v>0.00352524210794846</v>
-      </c>
-      <c r="F93" s="11" t="n">
+      <c r="D93" s="8" t="n">
+        <f aca="false">B93*D$47</f>
+        <v>0.01778816422549</v>
+      </c>
+      <c r="E93" s="8" t="n">
+        <f aca="false">B93*E$47</f>
+        <v>0.00353250258608168</v>
+      </c>
+      <c r="F93" s="10" t="n">
         <f aca="false">E93/D93</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G93" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G93" s="14" t="n">
         <f aca="false">E93-0.5*8*D93^2</f>
-        <v>0.00226394094173141</v>
+        <v>0.00226682744002967</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="10" t="n">
+      <c r="B94" s="8" t="n">
         <f aca="false">B93+0.02</f>
         <v>0.52</v>
       </c>
-      <c r="C94" s="10" t="n">
+      <c r="C94" s="8" t="n">
         <f aca="false">1-B94</f>
         <v>0.48</v>
       </c>
-      <c r="D94" s="10" t="n">
-        <f aca="false">B94*D$48</f>
-        <v>0.0184676970774671</v>
-      </c>
-      <c r="E94" s="10" t="n">
-        <f aca="false">B94*E$48</f>
-        <v>0.0036662517922664</v>
-      </c>
-      <c r="F94" s="11" t="n">
+      <c r="D94" s="8" t="n">
+        <f aca="false">B94*D$47</f>
+        <v>0.0184996907945096</v>
+      </c>
+      <c r="E94" s="8" t="n">
+        <f aca="false">B94*E$47</f>
+        <v>0.00367380268952495</v>
+      </c>
+      <c r="F94" s="10" t="n">
         <f aca="false">E94/D94</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G94" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G94" s="14" t="n">
         <f aca="false">E94-0.5*8*D94^2</f>
-        <v>0.00230202845088604</v>
+        <v>0.00230484845155509</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="10" t="n">
+      <c r="B95" s="8" t="n">
         <f aca="false">B94+0.02</f>
         <v>0.54</v>
       </c>
-      <c r="C95" s="10" t="n">
+      <c r="C95" s="8" t="n">
         <f aca="false">1-B95</f>
         <v>0.46</v>
       </c>
-      <c r="D95" s="10" t="n">
-        <f aca="false">B95*D$48</f>
-        <v>0.0191779931189082</v>
-      </c>
-      <c r="E95" s="10" t="n">
-        <f aca="false">B95*E$48</f>
-        <v>0.00380726147658433</v>
-      </c>
-      <c r="F95" s="11" t="n">
+      <c r="D95" s="8" t="n">
+        <f aca="false">B95*D$47</f>
+        <v>0.0192112173635292</v>
+      </c>
+      <c r="E95" s="8" t="n">
+        <f aca="false">B95*E$47</f>
+        <v>0.00381510279296821</v>
+      </c>
+      <c r="F95" s="10" t="n">
         <f aca="false">E95/D95</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G95" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G95" s="14" t="n">
         <f aca="false">E95-0.5*8*D95^2</f>
-        <v>0.00233607979630877</v>
+        <v>0.00233881930261315</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="10" t="n">
+      <c r="B96" s="8" t="n">
         <f aca="false">B95+0.02</f>
         <v>0.56</v>
       </c>
-      <c r="C96" s="10" t="n">
+      <c r="C96" s="8" t="n">
         <f aca="false">1-B96</f>
         <v>0.44</v>
       </c>
-      <c r="D96" s="10" t="n">
-        <f aca="false">B96*D$48</f>
-        <v>0.0198882891603492</v>
-      </c>
-      <c r="E96" s="10" t="n">
-        <f aca="false">B96*E$48</f>
-        <v>0.00394827116090227</v>
-      </c>
-      <c r="F96" s="11" t="n">
+      <c r="D96" s="8" t="n">
+        <f aca="false">B96*D$47</f>
+        <v>0.0199227439325488</v>
+      </c>
+      <c r="E96" s="8" t="n">
+        <f aca="false">B96*E$47</f>
+        <v>0.00395640289641148</v>
+      </c>
+      <c r="F96" s="10" t="n">
         <f aca="false">E96/D96</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G96" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G96" s="14" t="n">
         <f aca="false">E96-0.5*8*D96^2</f>
-        <v>0.00236609497799961</v>
+        <v>0.00236873999320384</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="10" t="n">
+      <c r="B97" s="8" t="n">
         <f aca="false">B96+0.02</f>
         <v>0.58</v>
       </c>
-      <c r="C97" s="10" t="n">
+      <c r="C97" s="8" t="n">
         <f aca="false">1-B97</f>
         <v>0.42</v>
       </c>
-      <c r="D97" s="10" t="n">
-        <f aca="false">B97*D$48</f>
-        <v>0.0205985852017903</v>
-      </c>
-      <c r="E97" s="10" t="n">
-        <f aca="false">B97*E$48</f>
-        <v>0.00408928084522021</v>
-      </c>
-      <c r="F97" s="11" t="n">
+      <c r="D97" s="8" t="n">
+        <f aca="false">B97*D$47</f>
+        <v>0.0206342705015684</v>
+      </c>
+      <c r="E97" s="8" t="n">
+        <f aca="false">B97*E$47</f>
+        <v>0.00409770299985475</v>
+      </c>
+      <c r="F97" s="10" t="n">
         <f aca="false">E97/D97</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G97" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G97" s="14" t="n">
         <f aca="false">E97-0.5*8*D97^2</f>
-        <v>0.00239207399595856</v>
+        <v>0.00239461052332717</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="10" t="n">
+      <c r="B98" s="8" t="n">
         <f aca="false">B97+0.02</f>
         <v>0.6</v>
       </c>
-      <c r="C98" s="10" t="n">
+      <c r="C98" s="8" t="n">
         <f aca="false">1-B98</f>
         <v>0.4</v>
       </c>
-      <c r="D98" s="10" t="n">
-        <f aca="false">B98*D$48</f>
-        <v>0.0213088812432313</v>
-      </c>
-      <c r="E98" s="10" t="n">
-        <f aca="false">B98*E$48</f>
-        <v>0.00423029052953815</v>
-      </c>
-      <c r="F98" s="11" t="n">
+      <c r="D98" s="8" t="n">
+        <f aca="false">B98*D$47</f>
+        <v>0.021345797070588</v>
+      </c>
+      <c r="E98" s="8" t="n">
+        <f aca="false">B98*E$47</f>
+        <v>0.00423900310329802</v>
+      </c>
+      <c r="F98" s="10" t="n">
         <f aca="false">E98/D98</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G98" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G98" s="14" t="n">
         <f aca="false">E98-0.5*8*D98^2</f>
-        <v>0.00241401685018561</v>
+        <v>0.00241643089298312</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="10" t="n">
+      <c r="B99" s="8" t="n">
         <f aca="false">B98+0.02</f>
         <v>0.62</v>
       </c>
-      <c r="C99" s="10" t="n">
+      <c r="C99" s="8" t="n">
         <f aca="false">1-B99</f>
         <v>0.38</v>
       </c>
-      <c r="D99" s="10" t="n">
-        <f aca="false">B99*D$48</f>
-        <v>0.0220191772846724</v>
-      </c>
-      <c r="E99" s="10" t="n">
-        <f aca="false">B99*E$48</f>
-        <v>0.00437130021385609</v>
-      </c>
-      <c r="F99" s="11" t="n">
+      <c r="D99" s="8" t="n">
+        <f aca="false">B99*D$47</f>
+        <v>0.0220573236396076</v>
+      </c>
+      <c r="E99" s="8" t="n">
+        <f aca="false">B99*E$47</f>
+        <v>0.00438030320674128</v>
+      </c>
+      <c r="F99" s="10" t="n">
         <f aca="false">E99/D99</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G99" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G99" s="14" t="n">
         <f aca="false">E99-0.5*8*D99^2</f>
-        <v>0.00243192354068076</v>
+        <v>0.00243420110217171</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="10" t="n">
+      <c r="B100" s="8" t="n">
         <f aca="false">B99+0.02</f>
         <v>0.64</v>
       </c>
-      <c r="C100" s="10" t="n">
+      <c r="C100" s="8" t="n">
         <f aca="false">1-B100</f>
         <v>0.36</v>
       </c>
-      <c r="D100" s="10" t="n">
-        <f aca="false">B100*D$48</f>
-        <v>0.0227294733261134</v>
-      </c>
-      <c r="E100" s="10" t="n">
-        <f aca="false">B100*E$48</f>
-        <v>0.00451230989817403</v>
-      </c>
-      <c r="F100" s="11" t="n">
+      <c r="D100" s="8" t="n">
+        <f aca="false">B100*D$47</f>
+        <v>0.0227688502086272</v>
+      </c>
+      <c r="E100" s="8" t="n">
+        <f aca="false">B100*E$47</f>
+        <v>0.00452160331018455</v>
+      </c>
+      <c r="F100" s="10" t="n">
         <f aca="false">E100/D100</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G100" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G100" s="14" t="n">
         <f aca="false">E100-0.5*8*D100^2</f>
-        <v>0.00244579406744402</v>
+        <v>0.00244792115089294</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="10" t="n">
+      <c r="B101" s="8" t="n">
         <f aca="false">B100+0.02</f>
         <v>0.66</v>
       </c>
-      <c r="C101" s="10" t="n">
+      <c r="C101" s="8" t="n">
         <f aca="false">1-B101</f>
         <v>0.34</v>
       </c>
-      <c r="D101" s="10" t="n">
-        <f aca="false">B101*D$48</f>
-        <v>0.0234397693675545</v>
-      </c>
-      <c r="E101" s="10" t="n">
-        <f aca="false">B101*E$48</f>
-        <v>0.00465331958249196</v>
-      </c>
-      <c r="F101" s="11" t="n">
+      <c r="D101" s="8" t="n">
+        <f aca="false">B101*D$47</f>
+        <v>0.0234803767776468</v>
+      </c>
+      <c r="E101" s="8" t="n">
+        <f aca="false">B101*E$47</f>
+        <v>0.00466290341362782</v>
+      </c>
+      <c r="F101" s="10" t="n">
         <f aca="false">E101/D101</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G101" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G101" s="14" t="n">
         <f aca="false">E101-0.5*8*D101^2</f>
-        <v>0.00245562843047539</v>
+        <v>0.0024575910391468</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="10" t="n">
+      <c r="B102" s="8" t="n">
         <f aca="false">B101+0.02</f>
         <v>0.68</v>
       </c>
-      <c r="C102" s="10" t="n">
+      <c r="C102" s="8" t="n">
         <f aca="false">1-B102</f>
         <v>0.32</v>
       </c>
-      <c r="D102" s="10" t="n">
-        <f aca="false">B102*D$48</f>
-        <v>0.0241500654089955</v>
-      </c>
-      <c r="E102" s="10" t="n">
-        <f aca="false">B102*E$48</f>
-        <v>0.0047943292668099</v>
-      </c>
-      <c r="F102" s="11" t="n">
+      <c r="D102" s="8" t="n">
+        <f aca="false">B102*D$47</f>
+        <v>0.0241919033466664</v>
+      </c>
+      <c r="E102" s="8" t="n">
+        <f aca="false">B102*E$47</f>
+        <v>0.00480420351707109</v>
+      </c>
+      <c r="F102" s="10" t="n">
         <f aca="false">E102/D102</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G102" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G102" s="14" t="n">
         <f aca="false">E102-0.5*8*D102^2</f>
-        <v>0.00246142662977486</v>
+        <v>0.00246321076693329</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="13" t="n">
+      <c r="B103" s="12" t="n">
         <f aca="false">B102+0.02</f>
         <v>0.7</v>
       </c>
-      <c r="C103" s="13" t="n">
+      <c r="C103" s="12" t="n">
         <f aca="false">1-B103</f>
         <v>0.3</v>
       </c>
-      <c r="D103" s="13" t="n">
-        <f aca="false">B103*D$48</f>
-        <v>0.0248603614504365</v>
-      </c>
-      <c r="E103" s="13" t="n">
-        <f aca="false">B103*E$48</f>
-        <v>0.00493533895112784</v>
-      </c>
-      <c r="F103" s="15" t="n">
+      <c r="D103" s="8" t="n">
+        <f aca="false">B103*D$47</f>
+        <v>0.024903429915686</v>
+      </c>
+      <c r="E103" s="8" t="n">
+        <f aca="false">B103*E$47</f>
+        <v>0.00494550362051435</v>
+      </c>
+      <c r="F103" s="13" t="n">
         <f aca="false">E103/D103</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G103" s="17" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G103" s="15" t="n">
         <f aca="false">E103-0.5*8*D103^2</f>
-        <v>0.00246318866534243</v>
+        <v>0.00246478033425241</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="10" t="n">
+      <c r="B104" s="8" t="n">
         <f aca="false">B103+0.02</f>
         <v>0.72</v>
       </c>
-      <c r="C104" s="10" t="n">
+      <c r="C104" s="8" t="n">
         <f aca="false">1-B104</f>
         <v>0.28</v>
       </c>
-      <c r="D104" s="10" t="n">
-        <f aca="false">B104*D$48</f>
-        <v>0.0255706574918776</v>
-      </c>
-      <c r="E104" s="10" t="n">
-        <f aca="false">B104*E$48</f>
-        <v>0.00507634863544578</v>
-      </c>
-      <c r="F104" s="11" t="n">
+      <c r="D104" s="8" t="n">
+        <f aca="false">B104*D$47</f>
+        <v>0.0256149564847056</v>
+      </c>
+      <c r="E104" s="8" t="n">
+        <f aca="false">B104*E$47</f>
+        <v>0.00508680372395762</v>
+      </c>
+      <c r="F104" s="10" t="n">
         <f aca="false">E104/D104</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G104" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G104" s="14" t="n">
         <f aca="false">E104-0.5*8*D104^2</f>
-        <v>0.00246091453717812</v>
+        <v>0.00246229974110417</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="10" t="n">
+      <c r="B105" s="8" t="n">
         <f aca="false">B104+0.02</f>
         <v>0.74</v>
       </c>
-      <c r="C105" s="10" t="n">
+      <c r="C105" s="8" t="n">
         <f aca="false">1-B105</f>
         <v>0.26</v>
       </c>
-      <c r="D105" s="10" t="n">
-        <f aca="false">B105*D$48</f>
-        <v>0.0262809535333186</v>
-      </c>
-      <c r="E105" s="10" t="n">
-        <f aca="false">B105*E$48</f>
-        <v>0.00521735831976372</v>
-      </c>
-      <c r="F105" s="11" t="n">
+      <c r="D105" s="8" t="n">
+        <f aca="false">B105*D$47</f>
+        <v>0.0263264830537252</v>
+      </c>
+      <c r="E105" s="8" t="n">
+        <f aca="false">B105*E$47</f>
+        <v>0.00522810382740089</v>
+      </c>
+      <c r="F105" s="10" t="n">
         <f aca="false">E105/D105</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G105" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G105" s="14" t="n">
         <f aca="false">E105-0.5*8*D105^2</f>
-        <v>0.0024546042452819</v>
+        <v>0.00245576898748857</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="10" t="n">
+      <c r="B106" s="8" t="n">
         <f aca="false">B105+0.02</f>
         <v>0.76</v>
       </c>
-      <c r="C106" s="10" t="n">
+      <c r="C106" s="8" t="n">
         <f aca="false">1-B106</f>
         <v>0.24</v>
       </c>
-      <c r="D106" s="10" t="n">
-        <f aca="false">B106*D$48</f>
-        <v>0.0269912495747597</v>
-      </c>
-      <c r="E106" s="10" t="n">
-        <f aca="false">B106*E$48</f>
-        <v>0.00535836800408166</v>
-      </c>
-      <c r="F106" s="11" t="n">
+      <c r="D106" s="8" t="n">
+        <f aca="false">B106*D$47</f>
+        <v>0.0270380096227448</v>
+      </c>
+      <c r="E106" s="8" t="n">
+        <f aca="false">B106*E$47</f>
+        <v>0.00536940393084415</v>
+      </c>
+      <c r="F106" s="10" t="n">
         <f aca="false">E106/D106</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G106" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G106" s="14" t="n">
         <f aca="false">E106-0.5*8*D106^2</f>
-        <v>0.0024442577896538</v>
+        <v>0.00244518807340559</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="10" t="n">
+      <c r="B107" s="8" t="n">
         <f aca="false">B106+0.02</f>
         <v>0.78</v>
       </c>
-      <c r="C107" s="10" t="n">
+      <c r="C107" s="8" t="n">
         <f aca="false">1-B107</f>
         <v>0.22</v>
       </c>
-      <c r="D107" s="10" t="n">
-        <f aca="false">B107*D$48</f>
-        <v>0.0277015456162007</v>
-      </c>
-      <c r="E107" s="10" t="n">
-        <f aca="false">B107*E$48</f>
-        <v>0.00549937768839959</v>
-      </c>
-      <c r="F107" s="11" t="n">
+      <c r="D107" s="8" t="n">
+        <f aca="false">B107*D$47</f>
+        <v>0.0277495361917644</v>
+      </c>
+      <c r="E107" s="8" t="n">
+        <f aca="false">B107*E$47</f>
+        <v>0.00551070403428742</v>
+      </c>
+      <c r="F107" s="10" t="n">
         <f aca="false">E107/D107</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G107" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G107" s="14" t="n">
         <f aca="false">E107-0.5*8*D107^2</f>
-        <v>0.0024298751702938</v>
+        <v>0.00243055699885525</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="10" t="n">
+      <c r="B108" s="8" t="n">
         <f aca="false">B107+0.02</f>
         <v>0.8</v>
       </c>
-      <c r="C108" s="10" t="n">
+      <c r="C108" s="8" t="n">
         <f aca="false">1-B108</f>
         <v>0.2</v>
       </c>
-      <c r="D108" s="10" t="n">
-        <f aca="false">B108*D$48</f>
-        <v>0.0284118416576418</v>
-      </c>
-      <c r="E108" s="10" t="n">
-        <f aca="false">B108*E$48</f>
-        <v>0.00564038737271753</v>
-      </c>
-      <c r="F108" s="11" t="n">
+      <c r="D108" s="8" t="n">
+        <f aca="false">B108*D$47</f>
+        <v>0.028461062760784</v>
+      </c>
+      <c r="E108" s="8" t="n">
+        <f aca="false">B108*E$47</f>
+        <v>0.00565200413773069</v>
+      </c>
+      <c r="F108" s="10" t="n">
         <f aca="false">E108/D108</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G108" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G108" s="14" t="n">
         <f aca="false">E108-0.5*8*D108^2</f>
-        <v>0.0024114563872019</v>
+        <v>0.00241187576383754</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="10" t="n">
+      <c r="B109" s="8" t="n">
         <f aca="false">B108+0.02</f>
         <v>0.82</v>
       </c>
-      <c r="C109" s="10" t="n">
+      <c r="C109" s="8" t="n">
         <f aca="false">1-B109</f>
         <v>0.18</v>
       </c>
-      <c r="D109" s="10" t="n">
-        <f aca="false">B109*D$48</f>
-        <v>0.0291221376990828</v>
-      </c>
-      <c r="E109" s="10" t="n">
-        <f aca="false">B109*E$48</f>
-        <v>0.00578139705703547</v>
-      </c>
-      <c r="F109" s="11" t="n">
+      <c r="D109" s="8" t="n">
+        <f aca="false">B109*D$47</f>
+        <v>0.0291725893298036</v>
+      </c>
+      <c r="E109" s="8" t="n">
+        <f aca="false">B109*E$47</f>
+        <v>0.00579330424117395</v>
+      </c>
+      <c r="F109" s="10" t="n">
         <f aca="false">E109/D109</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G109" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G109" s="14" t="n">
         <f aca="false">E109-0.5*8*D109^2</f>
-        <v>0.00238900144037811</v>
+        <v>0.00238914436835247</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="10" t="n">
+      <c r="B110" s="8" t="n">
         <f aca="false">B109+0.02</f>
         <v>0.84</v>
       </c>
-      <c r="C110" s="10" t="n">
+      <c r="C110" s="8" t="n">
         <f aca="false">1-B110</f>
         <v>0.16</v>
       </c>
-      <c r="D110" s="10" t="n">
-        <f aca="false">B110*D$48</f>
-        <v>0.0298324337405239</v>
-      </c>
-      <c r="E110" s="10" t="n">
-        <f aca="false">B110*E$48</f>
-        <v>0.00592240674135341</v>
-      </c>
-      <c r="F110" s="11" t="n">
+      <c r="D110" s="8" t="n">
+        <f aca="false">B110*D$47</f>
+        <v>0.0298841158988232</v>
+      </c>
+      <c r="E110" s="8" t="n">
+        <f aca="false">B110*E$47</f>
+        <v>0.00593460434461722</v>
+      </c>
+      <c r="F110" s="10" t="n">
         <f aca="false">E110/D110</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G110" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G110" s="14" t="n">
         <f aca="false">E110-0.5*8*D110^2</f>
-        <v>0.00236251032982242</v>
+        <v>0.00236236281240003</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="10" t="n">
+      <c r="B111" s="8" t="n">
         <f aca="false">B110+0.02</f>
         <v>0.86</v>
       </c>
-      <c r="C111" s="10" t="n">
+      <c r="C111" s="8" t="n">
         <f aca="false">1-B111</f>
         <v>0.14</v>
       </c>
-      <c r="D111" s="10" t="n">
-        <f aca="false">B111*D$48</f>
-        <v>0.0305427297819649</v>
-      </c>
-      <c r="E111" s="10" t="n">
-        <f aca="false">B111*E$48</f>
-        <v>0.00606341642567135</v>
-      </c>
-      <c r="F111" s="11" t="n">
+      <c r="D111" s="8" t="n">
+        <f aca="false">B111*D$47</f>
+        <v>0.0305956424678428</v>
+      </c>
+      <c r="E111" s="8" t="n">
+        <f aca="false">B111*E$47</f>
+        <v>0.00607590444806049</v>
+      </c>
+      <c r="F111" s="10" t="n">
         <f aca="false">E111/D111</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G111" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G111" s="14" t="n">
         <f aca="false">E111-0.5*8*D111^2</f>
-        <v>0.00233198305553485</v>
+        <v>0.00233153109598023</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="10" t="n">
+      <c r="B112" s="8" t="n">
         <f aca="false">B111+0.02</f>
         <v>0.88</v>
       </c>
-      <c r="C112" s="10" t="n">
+      <c r="C112" s="8" t="n">
         <f aca="false">1-B112</f>
         <v>0.12</v>
       </c>
-      <c r="D112" s="10" t="n">
-        <f aca="false">B112*D$48</f>
-        <v>0.0312530258234059</v>
-      </c>
-      <c r="E112" s="10" t="n">
-        <f aca="false">B112*E$48</f>
-        <v>0.00620442610998929</v>
-      </c>
-      <c r="F112" s="11" t="n">
+      <c r="D112" s="8" t="n">
+        <f aca="false">B112*D$47</f>
+        <v>0.0313071690368624</v>
+      </c>
+      <c r="E112" s="8" t="n">
+        <f aca="false">B112*E$47</f>
+        <v>0.00621720455150376</v>
+      </c>
+      <c r="F112" s="10" t="n">
         <f aca="false">E112/D112</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G112" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G112" s="14" t="n">
         <f aca="false">E112-0.5*8*D112^2</f>
-        <v>0.00229741961751537</v>
+        <v>0.00229664921909305</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="10" t="n">
+      <c r="B113" s="8" t="n">
         <f aca="false">B112+0.02</f>
         <v>0.9</v>
       </c>
-      <c r="C113" s="10" t="n">
+      <c r="C113" s="8" t="n">
         <f aca="false">1-B113</f>
         <v>0.0999999999999995</v>
       </c>
-      <c r="D113" s="10" t="n">
-        <f aca="false">B113*D$48</f>
-        <v>0.031963321864847</v>
-      </c>
-      <c r="E113" s="10" t="n">
-        <f aca="false">B113*E$48</f>
-        <v>0.00634543579430722</v>
-      </c>
-      <c r="F113" s="11" t="n">
+      <c r="D113" s="8" t="n">
+        <f aca="false">B113*D$47</f>
+        <v>0.032018695605882</v>
+      </c>
+      <c r="E113" s="8" t="n">
+        <f aca="false">B113*E$47</f>
+        <v>0.00635850465494702</v>
+      </c>
+      <c r="F113" s="10" t="n">
         <f aca="false">E113/D113</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G113" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G113" s="14" t="n">
         <f aca="false">E113-0.5*8*D113^2</f>
-        <v>0.002258820015764</v>
+        <v>0.00225771718173851</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="10" t="n">
+      <c r="B114" s="8" t="n">
         <f aca="false">B113+0.02</f>
         <v>0.92</v>
       </c>
-      <c r="C114" s="10" t="n">
+      <c r="C114" s="8" t="n">
         <f aca="false">1-B114</f>
         <v>0.0799999999999995</v>
       </c>
-      <c r="D114" s="10" t="n">
-        <f aca="false">B114*D$48</f>
-        <v>0.032673617906288</v>
-      </c>
-      <c r="E114" s="10" t="n">
-        <f aca="false">B114*E$48</f>
-        <v>0.00648644547862516</v>
-      </c>
-      <c r="F114" s="11" t="n">
+      <c r="D114" s="8" t="n">
+        <f aca="false">B114*D$47</f>
+        <v>0.0327302221749016</v>
+      </c>
+      <c r="E114" s="8" t="n">
+        <f aca="false">B114*E$47</f>
+        <v>0.00649980475839029</v>
+      </c>
+      <c r="F114" s="10" t="n">
         <f aca="false">E114/D114</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G114" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G114" s="14" t="n">
         <f aca="false">E114-0.5*8*D114^2</f>
-        <v>0.00221618425028074</v>
+        <v>0.00221473498391661</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="10" t="n">
+      <c r="B115" s="8" t="n">
         <f aca="false">B114+0.02</f>
         <v>0.94</v>
       </c>
-      <c r="C115" s="10" t="n">
+      <c r="C115" s="8" t="n">
         <f aca="false">1-B115</f>
         <v>0.0599999999999995</v>
       </c>
-      <c r="D115" s="10" t="n">
-        <f aca="false">B115*D$48</f>
-        <v>0.0333839139477291</v>
-      </c>
-      <c r="E115" s="10" t="n">
-        <f aca="false">B115*E$48</f>
-        <v>0.0066274551629431</v>
-      </c>
-      <c r="F115" s="11" t="n">
+      <c r="D115" s="8" t="n">
+        <f aca="false">B115*D$47</f>
+        <v>0.0334417487439212</v>
+      </c>
+      <c r="E115" s="8" t="n">
+        <f aca="false">B115*E$47</f>
+        <v>0.00664110486183356</v>
+      </c>
+      <c r="F115" s="10" t="n">
         <f aca="false">E115/D115</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G115" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G115" s="14" t="n">
         <f aca="false">E115-0.5*8*D115^2</f>
-        <v>0.00216951232106558</v>
+        <v>0.00216770262562734</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="10" t="n">
+      <c r="B116" s="8" t="n">
         <f aca="false">B115+0.02</f>
         <v>0.960000000000001</v>
       </c>
-      <c r="C116" s="10" t="n">
+      <c r="C116" s="8" t="n">
         <f aca="false">1-B116</f>
         <v>0.0399999999999995</v>
       </c>
-      <c r="D116" s="10" t="n">
-        <f aca="false">B116*D$48</f>
-        <v>0.0340942099891701</v>
-      </c>
-      <c r="E116" s="10" t="n">
-        <f aca="false">B116*E$48</f>
-        <v>0.00676846484726104</v>
-      </c>
-      <c r="F116" s="11" t="n">
+      <c r="D116" s="8" t="n">
+        <f aca="false">B116*D$47</f>
+        <v>0.0341532753129408</v>
+      </c>
+      <c r="E116" s="8" t="n">
+        <f aca="false">B116*E$47</f>
+        <v>0.00678240496527683</v>
+      </c>
+      <c r="F116" s="10" t="n">
         <f aca="false">E116/D116</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G116" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G116" s="14" t="n">
         <f aca="false">E116-0.5*8*D116^2</f>
-        <v>0.00211880422811853</v>
+        <v>0.0021166201068707</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="10" t="n">
+      <c r="B117" s="8" t="n">
         <f aca="false">B116+0.02</f>
         <v>0.98</v>
       </c>
-      <c r="C117" s="10" t="n">
+      <c r="C117" s="8" t="n">
         <f aca="false">1-B117</f>
         <v>0.0199999999999995</v>
       </c>
-      <c r="D117" s="10" t="n">
-        <f aca="false">B117*D$48</f>
-        <v>0.0348045060306112</v>
-      </c>
-      <c r="E117" s="10" t="n">
-        <f aca="false">B117*E$48</f>
-        <v>0.00690947453157898</v>
-      </c>
-      <c r="F117" s="11" t="n">
+      <c r="D117" s="8" t="n">
+        <f aca="false">B117*D$47</f>
+        <v>0.0348648018819604</v>
+      </c>
+      <c r="E117" s="8" t="n">
+        <f aca="false">B117*E$47</f>
+        <v>0.00692370506872009</v>
+      </c>
+      <c r="F117" s="10" t="n">
         <f aca="false">E117/D117</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G117" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G117" s="14" t="n">
         <f aca="false">E117-0.5*8*D117^2</f>
-        <v>0.00206405997143958</v>
+        <v>0.00206148742764669</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="10" t="n">
+      <c r="B118" s="8" t="n">
         <f aca="false">B117+0.02</f>
         <v>1</v>
       </c>
-      <c r="C118" s="10" t="n">
+      <c r="C118" s="8" t="n">
         <f aca="false">1-B118</f>
         <v>0</v>
       </c>
-      <c r="D118" s="10" t="n">
-        <f aca="false">B118*D$48</f>
-        <v>0.0355148020720522</v>
-      </c>
-      <c r="E118" s="10" t="n">
-        <f aca="false">B118*E$48</f>
-        <v>0.00705048421589692</v>
-      </c>
-      <c r="F118" s="11" t="n">
+      <c r="D118" s="8" t="n">
+        <f aca="false">B118*D$47</f>
+        <v>0.03557632845098</v>
+      </c>
+      <c r="E118" s="8" t="n">
+        <f aca="false">B118*E$47</f>
+        <v>0.00706500517216336</v>
+      </c>
+      <c r="F118" s="10" t="n">
         <f aca="false">E118/D118</f>
-        <v>0.198522413319183</v>
-      </c>
-      <c r="G118" s="16" t="n">
+        <v>0.198587248313105</v>
+      </c>
+      <c r="G118" s="14" t="n">
         <f aca="false">E118-0.5*8*D118^2</f>
-        <v>0.00200527955102874</v>
+        <v>0.00200230458795532</v>
       </c>
     </row>
   </sheetData>
@@ -27116,10 +27098,10 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27196,7 +27178,7 @@
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="18" t="n">
+      <c r="B5" s="16" t="n">
         <f aca="false">CORREL('Excess returns'!C3:C242,'Excess returns'!D3:D242)</f>
         <v>0.243900032789206</v>
       </c>
@@ -27205,13 +27187,13 @@
       <c r="A6" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="18" t="n">
+      <c r="B6" s="16" t="n">
         <f aca="false">B5*B4*C4</f>
         <v>0.000563107357015079</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="17" t="s">
         <v>23</v>
       </c>
     </row>
@@ -27251,9 +27233,9 @@
       <c r="E12" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="20" t="n">
+      <c r="F12" s="18" t="n">
         <f aca="false" t="array" ref="F12:G12">TRANSPOSE( MMULT( MINVERSE( F3:G4 ) , TRANSPOSE(B3:C3) ))</f>
-        <v>3.98477447098941</v>
+        <v>3.9847744709894</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>1.59153973684947</v>
@@ -27276,7 +27258,7 @@
       <c r="A14" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="10" t="n">
+      <c r="B14" s="8" t="n">
         <f aca="false">B12*B3+C12*C3</f>
         <v>0.00706500517216336</v>
       </c>
@@ -27292,7 +27274,7 @@
       <c r="A15" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="10" t="n">
+      <c r="B15" s="8" t="n">
         <f aca="false">SQRT(B12^2*B4^2 + C12^2*C4^2 + 2*B12*C12*B6)</f>
         <v>0.03557632845098</v>
       </c>
@@ -27321,7 +27303,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="17" t="s">
         <v>30</v>
       </c>
     </row>
@@ -27365,14 +27347,14 @@
       <c r="A24" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="10" t="n">
+      <c r="B24" s="8" t="n">
         <f aca="false">B23*B14</f>
         <v>0.00494550362051435</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="10" t="n">
+      <c r="F24" s="8" t="n">
         <f aca="false">F23*F14</f>
         <v>0.00493006262484752</v>
       </c>
@@ -27381,14 +27363,14 @@
       <c r="A25" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="10" t="n">
+      <c r="B25" s="8" t="n">
         <f aca="false">B23*B15</f>
         <v>0.024903429915686</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="10" t="n">
+      <c r="F25" s="8" t="n">
         <f aca="false">F23*F15</f>
         <v>0.024824540843809</v>
       </c>
@@ -27397,28 +27379,28 @@
       <c r="A26" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="16" t="n">
+      <c r="B26" s="14" t="n">
         <f aca="false">B24 - 0.5*B20*B25^2</f>
         <v>0.00246478033425242</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="16" t="n">
+      <c r="F26" s="14" t="n">
         <f aca="false">F24 - 0.5*B20*F25^2</f>
         <v>0.00246503131242376</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="17" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19"/>
+      <c r="A29" s="17"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="19" t="s">
         <v>37</v>
       </c>
     </row>
@@ -27471,7 +27453,7 @@
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.35"/>
   </cols>
@@ -27545,11 +27527,11 @@
         <v>4</v>
       </c>
       <c r="B7" s="0" t="n">
-        <f aca="false" t="array" ref="B7:D9">=MMULT( TRANSPOSE( 'Demeaned excess returns'!B3:D242) , 'Demeaned excess returns'!B3:D242) / 239</f>
+        <f aca="false" t="array" ref="B7:D9">MMULT( TRANSPOSE( 'Demeaned excess returns'!B3:D242) , 'Demeaned excess returns'!B3:D242) / 239</f>
         <v>0.00185165193206256</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0.000937484171293462</v>
+        <v>0.000937484171293463</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>0.00154424792294134</v>
@@ -27560,7 +27542,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>0.000937484171293462</v>
+        <v>0.000937484171293463</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0.00144605691083703</v>
@@ -27584,7 +27566,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="17" t="s">
         <v>41</v>
       </c>
     </row>
@@ -27659,7 +27641,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="17" t="s">
         <v>30</v>
       </c>
     </row>
@@ -27681,12 +27663,12 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="17" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19"/>
+      <c r="A27" s="17"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">

</xml_diff>